<commit_message>
deliq score values optimization method last trial
</commit_message>
<xml_diff>
--- a/src/results/data_deliq_scores.xlsx
+++ b/src/results/data_deliq_scores.xlsx
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.7420313610689769</v>
+        <v>0.7925373904460953</v>
       </c>
     </row>
     <row r="3">
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.9435505953144279</v>
+        <v>0.9923836931244895</v>
       </c>
     </row>
     <row r="4">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.8865990498657695</v>
+        <v>0.9538685792706206</v>
       </c>
     </row>
     <row r="5">
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.8477623109767461</v>
+        <v>0.8476201109767462</v>
       </c>
     </row>
     <row r="6">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9136569555614505</v>
+        <v>0.9766291175100404</v>
       </c>
     </row>
     <row r="7">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.8096375395316048</v>
+        <v>0.8527870111403643</v>
       </c>
     </row>
     <row r="8">
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.5745321678143384</v>
+        <v>0.5744743178143384</v>
       </c>
     </row>
     <row r="9">
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.5541257427313913</v>
+        <v>0.5537217427313912</v>
       </c>
     </row>
     <row r="10">
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.4934646900469028</v>
+        <v>0.4934422400469028</v>
       </c>
     </row>
     <row r="11">
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.9131571973167346</v>
+        <v>0.9694074318081948</v>
       </c>
     </row>
     <row r="12">
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" t="n">
-        <v>1.63825910084363</v>
+        <v>1.692604419621658</v>
       </c>
     </row>
     <row r="13">
@@ -2068,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.9040771447148165</v>
+        <v>0.9721752402978235</v>
       </c>
     </row>
     <row r="14">
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.8842465657503401</v>
+        <v>0.8841043657503401</v>
       </c>
     </row>
     <row r="15">
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" t="n">
-        <v>1.441979013060151</v>
+        <v>1.498358306430684</v>
       </c>
     </row>
     <row r="16">
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.458820102776905</v>
+        <v>0.457982052776905</v>
       </c>
     </row>
     <row r="17">
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="AJ17" t="n">
-        <v>0.5737538351717257</v>
+        <v>0.5737116851717258</v>
       </c>
     </row>
     <row r="18">
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" t="n">
-        <v>0.6403159648213056</v>
+        <v>0.6402567148213055</v>
       </c>
     </row>
     <row r="19">
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="AJ19" t="n">
-        <v>0.6879251054200574</v>
+        <v>0.6878076054200574</v>
       </c>
     </row>
     <row r="20">
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1.056907078962385</v>
+        <v>1.122050436715656</v>
       </c>
     </row>
     <row r="21">
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="AJ21" t="n">
-        <v>0.752491068144743</v>
+        <v>0.7940115170779454</v>
       </c>
     </row>
     <row r="22">
@@ -3162,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" t="n">
-        <v>0.4750844889380377</v>
+        <v>0.4749351389380377</v>
       </c>
     </row>
     <row r="23">
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="AJ23" t="n">
-        <v>0.4878158449107392</v>
+        <v>0.4877589449107392</v>
       </c>
     </row>
     <row r="24">
@@ -3406,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="AJ24" t="n">
-        <v>0.724151597861573</v>
+        <v>0.724129597861573</v>
       </c>
     </row>
     <row r="25">
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" t="n">
-        <v>0.5709524053160996</v>
+        <v>0.5709366053160996</v>
       </c>
     </row>
     <row r="26">
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" t="n">
-        <v>1.420542167934098</v>
+        <v>1.463705891459361</v>
       </c>
     </row>
     <row r="27">
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" t="n">
-        <v>0.7539074394394103</v>
+        <v>0.8144935214615044</v>
       </c>
     </row>
     <row r="28">
@@ -3894,7 +3894,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" t="n">
-        <v>0.8119248835806356</v>
+        <v>0.8119003835806357</v>
       </c>
     </row>
     <row r="29">
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" t="n">
-        <v>1.090291444170098</v>
+        <v>1.159270868958391</v>
       </c>
     </row>
     <row r="30">
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" t="n">
-        <v>0.8049720156253043</v>
+        <v>0.8598697457202481</v>
       </c>
     </row>
     <row r="31">
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" t="n">
-        <v>0.9749843676477146</v>
+        <v>1.029680316774951</v>
       </c>
     </row>
     <row r="32">
@@ -4382,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="AJ32" t="n">
-        <v>0.6684223198710209</v>
+        <v>0.6959912237283377</v>
       </c>
     </row>
     <row r="33">
@@ -4504,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="AJ33" t="n">
-        <v>0.518539706953802</v>
+        <v>0.518453206953802</v>
       </c>
     </row>
     <row r="34">
@@ -4626,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" t="n">
-        <v>0.8903053880462248</v>
+        <v>0.9520116205626161</v>
       </c>
     </row>
     <row r="35">
@@ -4748,7 +4748,7 @@
         <v>0</v>
       </c>
       <c r="AJ35" t="n">
-        <v>0.8987394106433729</v>
+        <v>0.9658244922144728</v>
       </c>
     </row>
     <row r="36">
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
       <c r="AJ36" t="n">
-        <v>0.9624034350360459</v>
+        <v>1.016288806548552</v>
       </c>
     </row>
     <row r="37">
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="AJ37" t="n">
-        <v>0.6389436885395416</v>
+        <v>0.6389225885395416</v>
       </c>
     </row>
     <row r="38">
@@ -5114,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="AJ38" t="n">
-        <v>0.8887674607326956</v>
+        <v>0.8886252607326957</v>
       </c>
     </row>
     <row r="39">
@@ -5236,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="AJ39" t="n">
-        <v>0.9016293766199324</v>
+        <v>0.9566470729316165</v>
       </c>
     </row>
     <row r="40">
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" t="n">
-        <v>0.7308441590109647</v>
+        <v>0.7306776590109646</v>
       </c>
     </row>
     <row r="41">
@@ -5480,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.6846724416075733</v>
+        <v>0.6846489416075733</v>
       </c>
     </row>
     <row r="42">
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="AJ42" t="n">
-        <v>0.9647931081765262</v>
+        <v>1.049748373761341</v>
       </c>
     </row>
     <row r="43">
@@ -5724,7 +5724,7 @@
         <v>0</v>
       </c>
       <c r="AJ43" t="n">
-        <v>0.9447540352731604</v>
+        <v>1.016478704912432</v>
       </c>
     </row>
     <row r="44">
@@ -5842,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="AJ44" t="n">
-        <v>0.4936414312763994</v>
+        <v>0.4934920812763994</v>
       </c>
     </row>
     <row r="45">
@@ -5964,7 +5964,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" t="n">
-        <v>0.984466674820954</v>
+        <v>1.044996899998732</v>
       </c>
     </row>
     <row r="46">
@@ -6086,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="AJ46" t="n">
-        <v>1.113484482260209</v>
+        <v>1.183982259576716</v>
       </c>
     </row>
     <row r="47">
@@ -6208,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="AJ47" t="n">
-        <v>0.6650136322000321</v>
+        <v>0.664280482200032</v>
       </c>
     </row>
     <row r="48">
@@ -6330,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" t="n">
-        <v>1.522966447707871</v>
+        <v>1.578028125533047</v>
       </c>
     </row>
     <row r="49">
@@ -6452,7 +6452,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" t="n">
-        <v>0.6536292279425454</v>
+        <v>0.6534586279425454</v>
       </c>
     </row>
     <row r="50">
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
       <c r="AJ50" t="n">
-        <v>0.4934790400469028</v>
+        <v>0.4934545400469028</v>
       </c>
     </row>
     <row r="51">
@@ -6696,7 +6696,7 @@
         <v>0</v>
       </c>
       <c r="AJ51" t="n">
-        <v>0.8208437632670869</v>
+        <v>0.8693633448586154</v>
       </c>
     </row>
     <row r="52">
@@ -6818,7 +6818,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" t="n">
-        <v>0.5793251351717258</v>
+        <v>0.5784870851717258</v>
       </c>
     </row>
     <row r="53">
@@ -6940,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="AJ53" t="n">
-        <v>0.720778188321561</v>
+        <v>0.7548198096938955</v>
       </c>
     </row>
     <row r="54">
@@ -7062,7 +7062,7 @@
         <v>0</v>
       </c>
       <c r="AJ54" t="n">
-        <v>0.4609360371216572</v>
+        <v>0.4608973871216572</v>
       </c>
     </row>
     <row r="55">
@@ -7184,7 +7184,7 @@
         <v>0</v>
       </c>
       <c r="AJ55" t="n">
-        <v>0.4741202389380377</v>
+        <v>0.4741086389380377</v>
       </c>
     </row>
     <row r="56">
@@ -7306,7 +7306,7 @@
         <v>0</v>
       </c>
       <c r="AJ56" t="n">
-        <v>0.4953814712167742</v>
+        <v>0.4953603712167742</v>
       </c>
     </row>
     <row r="57">
@@ -7428,7 +7428,7 @@
         <v>0</v>
       </c>
       <c r="AJ57" t="n">
-        <v>0.5493147594943232</v>
+        <v>0.5491441594943232</v>
       </c>
     </row>
     <row r="58">
@@ -7550,7 +7550,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" t="n">
-        <v>1.137842389343291</v>
+        <v>1.209228534529375</v>
       </c>
     </row>
     <row r="59">
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="AJ59" t="n">
-        <v>0.9063939520653459</v>
+        <v>0.9062517520653459</v>
       </c>
     </row>
     <row r="60">
@@ -7794,7 +7794,7 @@
         <v>0</v>
       </c>
       <c r="AJ60" t="n">
-        <v>1.085798330316885</v>
+        <v>1.154179464354207</v>
       </c>
     </row>
     <row r="61">
@@ -7916,7 +7916,7 @@
         <v>0</v>
       </c>
       <c r="AJ61" t="n">
-        <v>0.7900968668876256</v>
+        <v>0.8334780990825774</v>
       </c>
     </row>
     <row r="62">
@@ -8038,7 +8038,7 @@
         <v>0</v>
       </c>
       <c r="AJ62" t="n">
-        <v>0.683577110437702</v>
+        <v>0.683434910437702</v>
       </c>
     </row>
     <row r="63">
@@ -8160,7 +8160,7 @@
         <v>0</v>
       </c>
       <c r="AJ63" t="n">
-        <v>0.8293007449944628</v>
+        <v>0.877721102204935</v>
       </c>
     </row>
     <row r="64">
@@ -8278,7 +8278,7 @@
         <v>0</v>
       </c>
       <c r="AJ64" t="n">
-        <v>0.4780886038857703</v>
+        <v>0.4772505538857703</v>
       </c>
     </row>
     <row r="65">
@@ -8400,7 +8400,7 @@
         <v>0</v>
       </c>
       <c r="AJ65" t="n">
-        <v>0.9332012875189633</v>
+        <v>0.9330837875189633</v>
       </c>
     </row>
     <row r="66">
@@ -8522,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" t="n">
-        <v>0.9620649610642641</v>
+        <v>1.032685685891819</v>
       </c>
     </row>
     <row r="67">
@@ -8644,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="AJ67" t="n">
-        <v>0.5286101925480435</v>
+        <v>0.5284608425480435</v>
       </c>
     </row>
     <row r="68">
@@ -8766,7 +8766,7 @@
         <v>0</v>
       </c>
       <c r="AJ68" t="n">
-        <v>0.529662473717915</v>
+        <v>0.529637973717915</v>
       </c>
     </row>
     <row r="69">
@@ -8888,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="AJ69" t="n">
-        <v>0.909925278042772</v>
+        <v>0.9625011009970907</v>
       </c>
     </row>
     <row r="70">
@@ -9010,7 +9010,7 @@
         <v>0</v>
       </c>
       <c r="AJ70" t="n">
-        <v>0.8303139943463935</v>
+        <v>0.8302894943463935</v>
       </c>
     </row>
     <row r="71">
@@ -9132,7 +9132,7 @@
         <v>0</v>
       </c>
       <c r="AJ71" t="n">
-        <v>0.6131745414257253</v>
+        <v>0.6131422414257253</v>
       </c>
     </row>
     <row r="72">
@@ -9254,7 +9254,7 @@
         <v>0</v>
       </c>
       <c r="AJ72" t="n">
-        <v>0.5546982426795557</v>
+        <v>0.5545317426795556</v>
       </c>
     </row>
     <row r="73">
@@ -9376,7 +9376,7 @@
         <v>0</v>
       </c>
       <c r="AJ73" t="n">
-        <v>0.5286101925480435</v>
+        <v>0.5284608425480435</v>
       </c>
     </row>
     <row r="74">
@@ -9498,7 +9498,7 @@
         <v>0</v>
       </c>
       <c r="AJ74" t="n">
-        <v>0.6714894939095223</v>
+        <v>0.6710780939095223</v>
       </c>
     </row>
     <row r="75">
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="AJ75" t="n">
-        <v>0.5788362804493395</v>
+        <v>0.5787770304493395</v>
       </c>
     </row>
     <row r="76">
@@ -9742,7 +9742,7 @@
         <v>0</v>
       </c>
       <c r="AJ76" t="n">
-        <v>0.8570356671630065</v>
+        <v>0.9119019879321669</v>
       </c>
     </row>
     <row r="77">
@@ -9865,7 +9865,7 @@
         <v>0</v>
       </c>
       <c r="AJ77" t="n">
-        <v>0.8926684824371302</v>
+        <v>0.9413200973498507</v>
       </c>
     </row>
     <row r="78">
@@ -9987,7 +9987,7 @@
         <v>0</v>
       </c>
       <c r="AJ78" t="n">
-        <v>1.060561090604651</v>
+        <v>1.136532742823891</v>
       </c>
     </row>
     <row r="79">
@@ -10109,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AJ79" t="n">
-        <v>0.688448060437702</v>
+        <v>0.687610010437702</v>
       </c>
     </row>
     <row r="80">
@@ -10231,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="AJ80" t="n">
-        <v>0.9591527858946329</v>
+        <v>1.023357029158501</v>
       </c>
     </row>
     <row r="81">
@@ -10353,7 +10353,7 @@
         <v>0</v>
       </c>
       <c r="AJ81" t="n">
-        <v>0.7973181223605196</v>
+        <v>0.8510445695975998</v>
       </c>
     </row>
     <row r="82">
@@ -10475,7 +10475,7 @@
         <v>0</v>
       </c>
       <c r="AJ82" t="n">
-        <v>0.5774527490524715</v>
+        <v>0.5774060490524714</v>
       </c>
     </row>
     <row r="83">
@@ -10597,7 +10597,7 @@
         <v>0</v>
       </c>
       <c r="AJ83" t="n">
-        <v>0.961322313053267</v>
+        <v>0.9813529252973711</v>
       </c>
     </row>
     <row r="84">
@@ -10719,7 +10719,7 @@
         <v>0</v>
       </c>
       <c r="AJ84" t="n">
-        <v>0.8650974663418805</v>
+        <v>0.9190961582035315</v>
       </c>
     </row>
     <row r="85">
@@ -10841,7 +10841,7 @@
         <v>0</v>
       </c>
       <c r="AJ85" t="n">
-        <v>1.300430885379126</v>
+        <v>1.363273829147948</v>
       </c>
     </row>
     <row r="86">
@@ -10963,7 +10963,7 @@
         <v>0</v>
       </c>
       <c r="AJ86" t="n">
-        <v>1.484811321621042</v>
+        <v>1.552148596586929</v>
       </c>
     </row>
     <row r="87">
@@ -11085,7 +11085,7 @@
         <v>0</v>
       </c>
       <c r="AJ87" t="n">
-        <v>0.695581562100274</v>
+        <v>0.695439362100274</v>
       </c>
     </row>
     <row r="88">
@@ -11207,7 +11207,7 @@
         <v>0</v>
       </c>
       <c r="AJ88" t="n">
-        <v>0.9183153455827281</v>
+        <v>0.9614527671914875</v>
       </c>
     </row>
     <row r="89">
@@ -11329,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="AJ89" t="n">
-        <v>0.4934646900469028</v>
+        <v>0.4934422400469028</v>
       </c>
     </row>
     <row r="90">
@@ -11451,7 +11451,7 @@
         <v>0</v>
       </c>
       <c r="AJ90" t="n">
-        <v>0.8815612165230636</v>
+        <v>0.9456944767608589</v>
       </c>
     </row>
     <row r="91">
@@ -11573,7 +11573,7 @@
         <v>0</v>
       </c>
       <c r="AJ91" t="n">
-        <v>0.4643720916967175</v>
+        <v>0.4643496416967175</v>
       </c>
     </row>
     <row r="92">
@@ -11695,7 +11695,7 @@
         <v>0</v>
       </c>
       <c r="AJ92" t="n">
-        <v>1.085493852564391</v>
+        <v>1.133785606133643</v>
       </c>
     </row>
     <row r="93">
@@ -11817,7 +11817,7 @@
         <v>0</v>
       </c>
       <c r="AJ93" t="n">
-        <v>0.5498072152738173</v>
+        <v>0.5489691652738172</v>
       </c>
     </row>
     <row r="94">
@@ -11939,7 +11939,7 @@
         <v>0</v>
       </c>
       <c r="AJ94" t="n">
-        <v>0.5715056487498265</v>
+        <v>0.5714477987498265</v>
       </c>
     </row>
     <row r="95">
@@ -12061,7 +12061,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" t="n">
-        <v>1.151356957154473</v>
+        <v>1.151331207154473</v>
       </c>
     </row>
     <row r="96">
@@ -12183,7 +12183,7 @@
         <v>0</v>
       </c>
       <c r="AJ96" t="n">
-        <v>0.5177157376491537</v>
+        <v>0.5176072876491536</v>
       </c>
     </row>
     <row r="97">
@@ -12305,7 +12305,7 @@
         <v>0</v>
       </c>
       <c r="AJ97" t="n">
-        <v>0.5115987621647001</v>
+        <v>0.5114281621647001</v>
       </c>
     </row>
     <row r="98">
@@ -12427,7 +12427,7 @@
         <v>0</v>
       </c>
       <c r="AJ98" t="n">
-        <v>0.5690915867951569</v>
+        <v>0.5689422367951569</v>
       </c>
     </row>
     <row r="99">
@@ -12549,7 +12549,7 @@
         <v>0</v>
       </c>
       <c r="AJ99" t="n">
-        <v>0.8062118409213567</v>
+        <v>0.854846036501994</v>
       </c>
     </row>
     <row r="100">
@@ -12671,7 +12671,7 @@
         <v>0</v>
       </c>
       <c r="AJ100" t="n">
-        <v>0.6212656757704776</v>
+        <v>0.6211791757704777</v>
       </c>
     </row>
     <row r="101">
@@ -12793,7 +12793,7 @@
         <v>0</v>
       </c>
       <c r="AJ101" t="n">
-        <v>0.7170038972424654</v>
+        <v>0.7169446472424653</v>
       </c>
     </row>
     <row r="102">
@@ -12915,7 +12915,7 @@
         <v>0</v>
       </c>
       <c r="AJ102" t="n">
-        <v>0.8657610062626188</v>
+        <v>0.9142412960039988</v>
       </c>
     </row>
     <row r="103">
@@ -13037,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="AJ103" t="n">
-        <v>0.452337216162101</v>
+        <v>0.452281416162101</v>
       </c>
     </row>
     <row r="104">
@@ -13159,7 +13159,7 @@
         <v>0</v>
       </c>
       <c r="AJ104" t="n">
-        <v>0.5218743257839307</v>
+        <v>0.5210362757839306</v>
       </c>
     </row>
     <row r="105">
@@ -13281,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="AJ105" t="n">
-        <v>0.7729428630840864</v>
+        <v>0.80886799895221</v>
       </c>
     </row>
     <row r="106">
@@ -13403,7 +13403,7 @@
         <v>0</v>
       </c>
       <c r="AJ106" t="n">
-        <v>1.091934478757118</v>
+        <v>1.129912861801258</v>
       </c>
     </row>
     <row r="107">
@@ -13525,7 +13525,7 @@
         <v>0</v>
       </c>
       <c r="AJ107" t="n">
-        <v>0.5645946696571023</v>
+        <v>0.5644841196571023</v>
       </c>
     </row>
     <row r="108">
@@ -13647,7 +13647,7 @@
         <v>0</v>
       </c>
       <c r="AJ108" t="n">
-        <v>0.4665318371216572</v>
+        <v>0.4656937871216572</v>
       </c>
     </row>
     <row r="109">
@@ -13765,7 +13765,7 @@
         <v>0</v>
       </c>
       <c r="AJ109" t="n">
-        <v>0.600510893491741</v>
+        <v>0.600361543491741</v>
       </c>
     </row>
     <row r="110">
@@ -13887,7 +13887,7 @@
         <v>0</v>
       </c>
       <c r="AJ110" t="n">
-        <v>0.9611831816799867</v>
+        <v>1.004056651555323</v>
       </c>
     </row>
     <row r="111">
@@ -14009,7 +14009,7 @@
         <v>0</v>
       </c>
       <c r="AJ111" t="n">
-        <v>0.719744425711362</v>
+        <v>0.719573825711362</v>
       </c>
     </row>
     <row r="112">
@@ -14131,7 +14131,7 @@
         <v>0</v>
       </c>
       <c r="AJ112" t="n">
-        <v>1.051486177539763</v>
+        <v>1.118709085976296</v>
       </c>
     </row>
     <row r="113">
@@ -14253,7 +14253,7 @@
         <v>0</v>
       </c>
       <c r="AJ113" t="n">
-        <v>0.5780448922594406</v>
+        <v>0.5778783922594405</v>
       </c>
     </row>
     <row r="114">
@@ -14375,7 +14375,7 @@
         <v>0</v>
       </c>
       <c r="AJ114" t="n">
-        <v>0.9074861009446774</v>
+        <v>0.9726674402121934</v>
       </c>
     </row>
     <row r="115">
@@ -14498,7 +14498,7 @@
         <v>0</v>
       </c>
       <c r="AJ115" t="n">
-        <v>0.9209747760469624</v>
+        <v>0.9923111703348928</v>
       </c>
     </row>
     <row r="116">
@@ -14620,7 +14620,7 @@
         <v>0</v>
       </c>
       <c r="AJ116" t="n">
-        <v>0.5218743257839307</v>
+        <v>0.5210362757839306</v>
       </c>
     </row>
     <row r="117">
@@ -14742,7 +14742,7 @@
         <v>0</v>
       </c>
       <c r="AJ117" t="n">
-        <v>0.9946446215497307</v>
+        <v>1.065208408683048</v>
       </c>
     </row>
     <row r="118">
@@ -14864,7 +14864,7 @@
         <v>0</v>
       </c>
       <c r="AJ118" t="n">
-        <v>0.4073362483905605</v>
+        <v>0.4072769983905605</v>
       </c>
     </row>
     <row r="119">
@@ -14986,7 +14986,7 @@
         <v>0</v>
       </c>
       <c r="AJ119" t="n">
-        <v>0.8246539691064791</v>
+        <v>0.8723530651995517</v>
       </c>
     </row>
     <row r="120">
@@ -15108,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="AJ120" t="n">
-        <v>0.8472816379863223</v>
+        <v>0.9024456259694505</v>
       </c>
     </row>
     <row r="121">
@@ -15230,7 +15230,7 @@
         <v>0</v>
       </c>
       <c r="AJ121" t="n">
-        <v>0.458820102776905</v>
+        <v>0.457982052776905</v>
       </c>
     </row>
     <row r="122">
@@ -15352,7 +15352,7 @@
         <v>0</v>
       </c>
       <c r="AJ122" t="n">
-        <v>0.5917921578555171</v>
+        <v>0.5909541078555171</v>
       </c>
     </row>
     <row r="123">
@@ -15474,7 +15474,7 @@
         <v>0</v>
       </c>
       <c r="AJ123" t="n">
-        <v>0.9571195666805816</v>
+        <v>1.020556420737196</v>
       </c>
     </row>
     <row r="124">
@@ -15596,7 +15596,7 @@
         <v>0</v>
       </c>
       <c r="AJ124" t="n">
-        <v>0.5013409243916551</v>
+        <v>0.5012949743916552</v>
       </c>
     </row>
     <row r="125">
@@ -15719,7 +15719,7 @@
         <v>0</v>
       </c>
       <c r="AJ125" t="n">
-        <v>0.5669412508269736</v>
+        <v>0.5667706508269735</v>
       </c>
     </row>
     <row r="126">
@@ -15842,7 +15842,7 @@
         <v>0</v>
       </c>
       <c r="AJ126" t="n">
-        <v>1.019279990915378</v>
+        <v>1.099844942089622</v>
       </c>
     </row>
     <row r="127">
@@ -15964,7 +15964,7 @@
         <v>0</v>
       </c>
       <c r="AJ127" t="n">
-        <v>0.7797874270646756</v>
+        <v>0.8292806328643229</v>
       </c>
     </row>
     <row r="128">
@@ -16086,7 +16086,7 @@
         <v>0</v>
       </c>
       <c r="AJ128" t="n">
-        <v>0.7343844116852916</v>
+        <v>0.7343624116852916</v>
       </c>
     </row>
     <row r="129">
@@ -16208,7 +16208,7 @@
         <v>0</v>
       </c>
       <c r="AJ129" t="n">
-        <v>0.5651896822200968</v>
+        <v>0.5650906822200967</v>
       </c>
     </row>
     <row r="130">
@@ -16330,7 +16330,7 @@
         <v>0</v>
       </c>
       <c r="AJ130" t="n">
-        <v>0.5011960467271196</v>
+        <v>0.5011381967271197</v>
       </c>
     </row>
     <row r="131">
@@ -16452,7 +16452,7 @@
         <v>0</v>
       </c>
       <c r="AJ131" t="n">
-        <v>0.9680100425268977</v>
+        <v>1.016687616547627</v>
       </c>
     </row>
     <row r="132">
@@ -16574,7 +16574,7 @@
         <v>0</v>
       </c>
       <c r="AJ132" t="n">
-        <v>0.5141625914391784</v>
+        <v>0.5133245414391784</v>
       </c>
     </row>
     <row r="133">
@@ -16696,7 +16696,7 @@
         <v>0</v>
       </c>
       <c r="AJ133" t="n">
-        <v>0.9554307890968929</v>
+        <v>1.032535690400309</v>
       </c>
     </row>
     <row r="134">
@@ -16818,7 +16818,7 @@
         <v>0</v>
       </c>
       <c r="AJ134" t="n">
-        <v>1.255039129374555</v>
+        <v>1.312281891197334</v>
       </c>
     </row>
     <row r="135">
@@ -16940,7 +16940,7 @@
         <v>0</v>
       </c>
       <c r="AJ135" t="n">
-        <v>1.250489862402814</v>
+        <v>1.304241346694348</v>
       </c>
     </row>
     <row r="136">
@@ -17062,7 +17062,7 @@
         <v>0</v>
       </c>
       <c r="AJ136" t="n">
-        <v>0.6853528948349202</v>
+        <v>0.7192174240740079</v>
       </c>
     </row>
     <row r="137">
@@ -17184,7 +17184,7 @@
         <v>0</v>
       </c>
       <c r="AJ137" t="n">
-        <v>1.231228873264928</v>
+        <v>1.292094886049719</v>
       </c>
     </row>
     <row r="138">
@@ -17306,7 +17306,7 @@
         <v>0</v>
       </c>
       <c r="AJ138" t="n">
-        <v>0.6366729544756047</v>
+        <v>0.65672585354028</v>
       </c>
     </row>
     <row r="139">
@@ -17428,7 +17428,7 @@
         <v>0</v>
       </c>
       <c r="AJ139" t="n">
-        <v>1.119876358218554</v>
+        <v>1.180401383396333</v>
       </c>
     </row>
     <row r="140">
@@ -17550,7 +17550,7 @@
         <v>0</v>
       </c>
       <c r="AJ140" t="n">
-        <v>0.9514706286926625</v>
+        <v>1.011018668421963</v>
       </c>
     </row>
     <row r="141">
@@ -17672,7 +17672,7 @@
         <v>0</v>
       </c>
       <c r="AJ141" t="n">
-        <v>0.5600973251927344</v>
+        <v>0.5599479751927343</v>
       </c>
     </row>
     <row r="142">
@@ -17794,7 +17794,7 @@
         <v>0</v>
       </c>
       <c r="AJ142" t="n">
-        <v>0.4752562350556416</v>
+        <v>0.4750979850556415</v>
       </c>
     </row>
     <row r="143">
@@ -17916,7 +17916,7 @@
         <v>0</v>
       </c>
       <c r="AJ143" t="n">
-        <v>0.8527858699847422</v>
+        <v>0.8959180832627224</v>
       </c>
     </row>
     <row r="144">
@@ -18038,7 +18038,7 @@
         <v>0</v>
       </c>
       <c r="AJ144" t="n">
-        <v>0.9642302378961504</v>
+        <v>1.022290691461426</v>
       </c>
     </row>
     <row r="145">
@@ -18160,7 +18160,7 @@
         <v>0</v>
       </c>
       <c r="AJ145" t="n">
-        <v>1.234648434791128</v>
+        <v>1.298894681509867</v>
       </c>
     </row>
     <row r="146">
@@ -18282,7 +18282,7 @@
         <v>0</v>
       </c>
       <c r="AJ146" t="n">
-        <v>0.6392107385395417</v>
+        <v>0.6391514885395416</v>
       </c>
     </row>
     <row r="147">
@@ -18404,7 +18404,7 @@
         <v>0</v>
       </c>
       <c r="AJ147" t="n">
-        <v>0.5586065131136027</v>
+        <v>0.5584571631136026</v>
       </c>
     </row>
     <row r="148">
@@ -18526,7 +18526,7 @@
         <v>0</v>
       </c>
       <c r="AJ148" t="n">
-        <v>0.9304721233154412</v>
+        <v>0.9927056525554573</v>
       </c>
     </row>
     <row r="149">
@@ -18648,7 +18648,7 @@
         <v>0</v>
       </c>
       <c r="AJ149" t="n">
-        <v>0.5388483620989363</v>
+        <v>0.5387493620989362</v>
       </c>
     </row>
     <row r="150">
@@ -18770,7 +18770,7 @@
         <v>0</v>
       </c>
       <c r="AJ150" t="n">
-        <v>0.8945816473237302</v>
+        <v>0.9597242146484091</v>
       </c>
     </row>
     <row r="151">
@@ -18892,7 +18892,7 @@
         <v>0</v>
       </c>
       <c r="AJ151" t="n">
-        <v>0.5714746053160996</v>
+        <v>0.5713842053160997</v>
       </c>
     </row>
     <row r="152">
@@ -19014,7 +19014,7 @@
         <v>0</v>
       </c>
       <c r="AJ152" t="n">
-        <v>0.5715379553160996</v>
+        <v>0.5714385053160996</v>
       </c>
     </row>
     <row r="153">
@@ -19136,7 +19136,7 @@
         <v>0</v>
       </c>
       <c r="AJ153" t="n">
-        <v>1.156109790198289</v>
+        <v>1.232697303836056</v>
       </c>
     </row>
     <row r="154">
@@ -19258,7 +19258,7 @@
         <v>0</v>
       </c>
       <c r="AJ154" t="n">
-        <v>0.9548827629976921</v>
+        <v>1.008649783030582</v>
       </c>
     </row>
     <row r="155">
@@ -19380,7 +19380,7 @@
         <v>0</v>
       </c>
       <c r="AJ155" t="n">
-        <v>0.7299651010364541</v>
+        <v>0.7299391010364541</v>
       </c>
     </row>
     <row r="156">
@@ -19502,7 +19502,7 @@
         <v>0</v>
       </c>
       <c r="AJ156" t="n">
-        <v>1.139565841613164</v>
+        <v>1.182154006773891</v>
       </c>
     </row>
     <row r="157">
@@ -19624,7 +19624,7 @@
         <v>0</v>
       </c>
       <c r="AJ157" t="n">
-        <v>0.8453661377871359</v>
+        <v>0.8955210914472896</v>
       </c>
     </row>
     <row r="158">
@@ -19746,7 +19746,7 @@
         <v>0</v>
       </c>
       <c r="AJ158" t="n">
-        <v>0.4930009312763994</v>
+        <v>0.4929430812763994</v>
       </c>
     </row>
     <row r="159">
@@ -19868,7 +19868,7 @@
         <v>0</v>
       </c>
       <c r="AJ159" t="n">
-        <v>0.6956368397648095</v>
+        <v>0.6955193397648095</v>
       </c>
     </row>
     <row r="160">
@@ -19990,7 +19990,7 @@
         <v>0</v>
       </c>
       <c r="AJ160" t="n">
-        <v>0.480158433342415</v>
+        <v>0.480009083342415</v>
       </c>
     </row>
     <row r="161">
@@ -20112,7 +20112,7 @@
         <v>0</v>
       </c>
       <c r="AJ161" t="n">
-        <v>1.21731517069691</v>
+        <v>1.21721507069691</v>
       </c>
     </row>
     <row r="162">
@@ -20234,7 +20234,7 @@
         <v>0</v>
       </c>
       <c r="AJ162" t="n">
-        <v>0.9136316883158067</v>
+        <v>0.968378915642224</v>
       </c>
     </row>
     <row r="163">
@@ -20356,7 +20356,7 @@
         <v>0</v>
       </c>
       <c r="AJ163" t="n">
-        <v>1.196821814389742</v>
+        <v>1.259174966413742</v>
       </c>
     </row>
     <row r="164">
@@ -20478,7 +20478,7 @@
         <v>0</v>
       </c>
       <c r="AJ164" t="n">
-        <v>0.9641641144555391</v>
+        <v>1.030748053161446</v>
       </c>
     </row>
     <row r="165">
@@ -20600,7 +20600,7 @@
         <v>0</v>
       </c>
       <c r="AJ165" t="n">
-        <v>1.028202379685419</v>
+        <v>1.076561569979037</v>
       </c>
     </row>
     <row r="166">
@@ -20722,7 +20722,7 @@
         <v>0</v>
       </c>
       <c r="AJ166" t="n">
-        <v>1.194420947132834</v>
+        <v>1.24317055395123</v>
       </c>
     </row>
     <row r="167">
@@ -20840,7 +20840,7 @@
         <v>0</v>
       </c>
       <c r="AJ167" t="n">
-        <v>1.883655442365023</v>
+        <v>1.964031655474045</v>
       </c>
     </row>
     <row r="168">
@@ -20962,7 +20962,7 @@
         <v>0</v>
       </c>
       <c r="AJ168" t="n">
-        <v>0.967269924611135</v>
+        <v>1.038235879314084</v>
       </c>
     </row>
     <row r="169">
@@ -21084,7 +21084,7 @@
         <v>0</v>
       </c>
       <c r="AJ169" t="n">
-        <v>0.993120089736287</v>
+        <v>1.062314801659158</v>
       </c>
     </row>
     <row r="170">
@@ -21206,7 +21206,7 @@
         <v>0</v>
       </c>
       <c r="AJ170" t="n">
-        <v>1.199460385699354</v>
+        <v>1.261940642036995</v>
       </c>
     </row>
     <row r="171">
@@ -21324,7 +21324,7 @@
         <v>0</v>
       </c>
       <c r="AJ171" t="n">
-        <v>0.8190977433629275</v>
+        <v>0.8672474105628644</v>
       </c>
     </row>
     <row r="172">
@@ -21446,7 +21446,7 @@
         <v>0</v>
       </c>
       <c r="AJ172" t="n">
-        <v>0.8495247363754226</v>
+        <v>0.8921349857185163</v>
       </c>
     </row>
     <row r="173">
@@ -21568,7 +21568,7 @@
         <v>0</v>
       </c>
       <c r="AJ173" t="n">
-        <v>1.034911059726127</v>
+        <v>1.116409022090248</v>
       </c>
     </row>
     <row r="174">
@@ -21690,7 +21690,7 @@
         <v>0</v>
       </c>
       <c r="AJ174" t="n">
-        <v>1.009941057150111</v>
+        <v>1.087295464193757</v>
       </c>
     </row>
     <row r="175">
@@ -21808,7 +21808,7 @@
         <v>0</v>
       </c>
       <c r="AJ175" t="n">
-        <v>1.020391763457603</v>
+        <v>1.092287690887407</v>
       </c>
     </row>
     <row r="176">
@@ -21930,7 +21930,7 @@
         <v>0</v>
       </c>
       <c r="AJ176" t="n">
-        <v>0.4807694997875926</v>
+        <v>0.4807584997875926</v>
       </c>
     </row>
     <row r="177">
@@ -22052,7 +22052,7 @@
         <v>0</v>
       </c>
       <c r="AJ177" t="n">
-        <v>0.9575572625101998</v>
+        <v>1.028678649568016</v>
       </c>
     </row>
     <row r="178">
@@ -22174,7 +22174,7 @@
         <v>0</v>
       </c>
       <c r="AJ178" t="n">
-        <v>0.8611865947337772</v>
+        <v>0.8611104947337772</v>
       </c>
     </row>
     <row r="179">
@@ -22296,7 +22296,7 @@
         <v>0</v>
       </c>
       <c r="AJ179" t="n">
-        <v>0.9880574942532051</v>
+        <v>1.042644113511559</v>
       </c>
     </row>
     <row r="180">
@@ -22418,7 +22418,7 @@
         <v>0</v>
       </c>
       <c r="AJ180" t="n">
-        <v>1.058893875392111</v>
+        <v>1.114794697415507</v>
       </c>
     </row>
     <row r="181">
@@ -22540,7 +22540,7 @@
         <v>0</v>
       </c>
       <c r="AJ181" t="n">
-        <v>1.182767017275836</v>
+        <v>1.264143300937408</v>
       </c>
     </row>
     <row r="182">
@@ -22662,7 +22662,7 @@
         <v>0</v>
       </c>
       <c r="AJ182" t="n">
-        <v>0.8687147744553939</v>
+        <v>0.9180126324793884</v>
       </c>
     </row>
     <row r="183">
@@ -22784,7 +22784,7 @@
         <v>0</v>
       </c>
       <c r="AJ183" t="n">
-        <v>0.5497607270829753</v>
+        <v>0.5493493270829753</v>
       </c>
     </row>
     <row r="184">
@@ -22906,7 +22906,7 @@
         <v>0</v>
       </c>
       <c r="AJ184" t="n">
-        <v>0.8295224047172409</v>
+        <v>0.8781943521778173</v>
       </c>
     </row>
     <row r="185">
@@ -23028,7 +23028,7 @@
         <v>0</v>
       </c>
       <c r="AJ185" t="n">
-        <v>0.6856005029077903</v>
+        <v>0.6855703529077903</v>
       </c>
     </row>
     <row r="186">
@@ -23150,7 +23150,7 @@
         <v>0</v>
       </c>
       <c r="AJ186" t="n">
-        <v>1.202818446278229</v>
+        <v>1.283394355303417</v>
       </c>
     </row>
     <row r="187">
@@ -23272,7 +23272,7 @@
         <v>0</v>
       </c>
       <c r="AJ187" t="n">
-        <v>0.9016929768237305</v>
+        <v>0.9516693443073232</v>
       </c>
     </row>
     <row r="188">
@@ -23394,7 +23394,7 @@
         <v>0</v>
       </c>
       <c r="AJ188" t="n">
-        <v>0.5697918423685485</v>
+        <v>0.5693804423685486</v>
       </c>
     </row>
     <row r="189">
@@ -23516,7 +23516,7 @@
         <v>0</v>
       </c>
       <c r="AJ189" t="n">
-        <v>0.9887876783462168</v>
+        <v>1.037143462269946</v>
       </c>
     </row>
     <row r="190">
@@ -23638,7 +23638,7 @@
         <v>0</v>
       </c>
       <c r="AJ190" t="n">
-        <v>0.6623659792678768</v>
+        <v>0.6620406292678768</v>
       </c>
     </row>
     <row r="191">
@@ -23760,7 +23760,7 @@
         <v>0</v>
       </c>
       <c r="AJ191" t="n">
-        <v>0.9264440678755372</v>
+        <v>0.9845834376587046</v>
       </c>
     </row>
     <row r="192">
@@ -23878,7 +23878,7 @@
         <v>0</v>
       </c>
       <c r="AJ192" t="n">
-        <v>0.9025213691062624</v>
+        <v>0.962124720927151</v>
       </c>
     </row>
     <row r="193">
@@ -24000,7 +24000,7 @@
         <v>0</v>
       </c>
       <c r="AJ193" t="n">
-        <v>1.548134589327775</v>
+        <v>1.603139258297761</v>
       </c>
     </row>
     <row r="194">
@@ -24122,7 +24122,7 @@
         <v>0</v>
       </c>
       <c r="AJ194" t="n">
-        <v>0.9462317804297625</v>
+        <v>0.994993339245444</v>
       </c>
     </row>
     <row r="195">
@@ -24244,7 +24244,7 @@
         <v>0</v>
       </c>
       <c r="AJ195" t="n">
-        <v>1.171275909539157</v>
+        <v>1.219961243335304</v>
       </c>
     </row>
     <row r="196">
@@ -24366,7 +24366,7 @@
         <v>0</v>
       </c>
       <c r="AJ196" t="n">
-        <v>1.11588881711257</v>
+        <v>1.151849702980694</v>
       </c>
     </row>
     <row r="197">
@@ -24488,7 +24488,7 @@
         <v>0</v>
       </c>
       <c r="AJ197" t="n">
-        <v>0.7590331667839063</v>
+        <v>0.7959827745004382</v>
       </c>
     </row>
     <row r="198">
@@ -24610,7 +24610,7 @@
         <v>0</v>
       </c>
       <c r="AJ198" t="n">
-        <v>0.888909448090878</v>
+        <v>0.9092042553966562</v>
       </c>
     </row>
     <row r="199">
@@ -24732,7 +24732,7 @@
         <v>0</v>
       </c>
       <c r="AJ199" t="n">
-        <v>1.118862792035758</v>
+        <v>1.179243524875816</v>
       </c>
     </row>
     <row r="200">
@@ -24854,7 +24854,7 @@
         <v>0</v>
       </c>
       <c r="AJ200" t="n">
-        <v>0.6077829270965198</v>
+        <v>0.6073260270965198</v>
       </c>
     </row>
     <row r="201">
@@ -24976,7 +24976,7 @@
         <v>0</v>
       </c>
       <c r="AJ201" t="n">
-        <v>0.9874170447594449</v>
+        <v>1.04076385723445</v>
       </c>
     </row>
     <row r="202">
@@ -25098,7 +25098,7 @@
         <v>0</v>
       </c>
       <c r="AJ202" t="n">
-        <v>0.7306303219245447</v>
+        <v>0.7500670799655079</v>
       </c>
     </row>
     <row r="203">
@@ -25220,7 +25220,7 @@
         <v>0</v>
       </c>
       <c r="AJ203" t="n">
-        <v>0.6126013798088261</v>
+        <v>0.6124765298088261</v>
       </c>
     </row>
     <row r="204">
@@ -25342,7 +25342,7 @@
         <v>0</v>
       </c>
       <c r="AJ204" t="n">
-        <v>1.23599743507572</v>
+        <v>1.311939934839388</v>
       </c>
     </row>
     <row r="205">
@@ -25464,7 +25464,7 @@
         <v>0</v>
       </c>
       <c r="AJ205" t="n">
-        <v>0.9276214220108981</v>
+        <v>0.9914017713695138</v>
       </c>
     </row>
     <row r="206">
@@ -25586,7 +25586,7 @@
         <v>0</v>
       </c>
       <c r="AJ206" t="n">
-        <v>0.7342626705987617</v>
+        <v>0.7767419092088824</v>
       </c>
     </row>
     <row r="207">
@@ -25708,7 +25708,7 @@
         <v>0</v>
       </c>
       <c r="AJ207" t="n">
-        <v>1.100432778281179</v>
+        <v>1.177566775237284</v>
       </c>
     </row>
     <row r="208">
@@ -25830,7 +25830,7 @@
         <v>0</v>
       </c>
       <c r="AJ208" t="n">
-        <v>0.779119487543341</v>
+        <v>0.8274137366686145</v>
       </c>
     </row>
     <row r="209">
@@ -25952,7 +25952,7 @@
         <v>0</v>
       </c>
       <c r="AJ209" t="n">
-        <v>0.8805393111611128</v>
+        <v>0.941324172998566</v>
       </c>
     </row>
     <row r="210">
@@ -26074,7 +26074,7 @@
         <v>0</v>
       </c>
       <c r="AJ210" t="n">
-        <v>1.22659773824993</v>
+        <v>1.308913371664553</v>
       </c>
     </row>
     <row r="211">
@@ -26196,7 +26196,7 @@
         <v>0</v>
       </c>
       <c r="AJ211" t="n">
-        <v>1.012682836487884</v>
+        <v>1.093586358015153</v>
       </c>
     </row>
     <row r="212">
@@ -26318,7 +26318,7 @@
         <v>0</v>
       </c>
       <c r="AJ212" t="n">
-        <v>0.7049085047272184</v>
+        <v>0.7048679547272184</v>
       </c>
     </row>
     <row r="213">
@@ -26440,7 +26440,7 @@
         <v>0</v>
       </c>
       <c r="AJ213" t="n">
-        <v>0.9947205060597738</v>
+        <v>1.043246314175693</v>
       </c>
     </row>
     <row r="214">
@@ -26562,7 +26562,7 @@
         <v>0</v>
       </c>
       <c r="AJ214" t="n">
-        <v>0.5756197147498241</v>
+        <v>0.5752083147498241</v>
       </c>
     </row>
     <row r="215">
@@ -26684,7 +26684,7 @@
         <v>0</v>
       </c>
       <c r="AJ215" t="n">
-        <v>0.7114168395854424</v>
+        <v>0.7664756922205411</v>
       </c>
     </row>
     <row r="216">
@@ -26806,7 +26806,7 @@
         <v>0</v>
       </c>
       <c r="AJ216" t="n">
-        <v>0.842873648782657</v>
+        <v>0.8427993487826571</v>
       </c>
     </row>
     <row r="217">
@@ -26928,7 +26928,7 @@
         <v>0</v>
       </c>
       <c r="AJ217" t="n">
-        <v>1.353244425384263</v>
+        <v>1.401781574360845</v>
       </c>
     </row>
     <row r="218">
@@ -27050,7 +27050,7 @@
         <v>0</v>
       </c>
       <c r="AJ218" t="n">
-        <v>0.851388007295965</v>
+        <v>0.8947324135308016</v>
       </c>
     </row>
     <row r="219">
@@ -27172,7 +27172,7 @@
         <v>0</v>
       </c>
       <c r="AJ219" t="n">
-        <v>0.7558309656798284</v>
+        <v>0.8040888728153683</v>
       </c>
     </row>
     <row r="220">
@@ -27294,7 +27294,7 @@
         <v>0</v>
       </c>
       <c r="AJ220" t="n">
-        <v>1.037954417086616</v>
+        <v>1.072011744695874</v>
       </c>
     </row>
     <row r="221">
@@ -27416,7 +27416,7 @@
         <v>0</v>
       </c>
       <c r="AJ221" t="n">
-        <v>0.8585953082861602</v>
+        <v>0.8585762082861601</v>
       </c>
     </row>
     <row r="222">
@@ -27538,7 +27538,7 @@
         <v>0</v>
       </c>
       <c r="AJ222" t="n">
-        <v>0.790547770795282</v>
+        <v>0.8107516240320719</v>
       </c>
     </row>
     <row r="223">
@@ -27660,7 +27660,7 @@
         <v>0</v>
       </c>
       <c r="AJ223" t="n">
-        <v>0.8522386256082558</v>
+        <v>0.9049752658979798</v>
       </c>
     </row>
     <row r="224">
@@ -27782,7 +27782,7 @@
         <v>0</v>
       </c>
       <c r="AJ224" t="n">
-        <v>0.8887928838562392</v>
+        <v>0.9517456958048289</v>
       </c>
     </row>
     <row r="225">
@@ -27904,7 +27904,7 @@
         <v>0</v>
       </c>
       <c r="AJ225" t="n">
-        <v>1.171279231358101</v>
+        <v>1.225069473655116</v>
       </c>
     </row>
     <row r="226">
@@ -28026,7 +28026,7 @@
         <v>0</v>
       </c>
       <c r="AJ226" t="n">
-        <v>1.235232645048596</v>
+        <v>1.28991781430695</v>
       </c>
     </row>
     <row r="227">
@@ -28144,7 +28144,7 @@
         <v>0</v>
       </c>
       <c r="AJ227" t="n">
-        <v>1.387154920645439</v>
+        <v>1.453744239061178</v>
       </c>
     </row>
     <row r="228">
@@ -28266,7 +28266,7 @@
         <v>0</v>
       </c>
       <c r="AJ228" t="n">
-        <v>1.270068586638994</v>
+        <v>1.270020136638994</v>
       </c>
     </row>
     <row r="229">
@@ -28388,7 +28388,7 @@
         <v>0</v>
       </c>
       <c r="AJ229" t="n">
-        <v>1.087383670858504</v>
+        <v>1.158599945218142</v>
       </c>
     </row>
     <row r="230">
@@ -28506,7 +28506,7 @@
         <v>0</v>
       </c>
       <c r="AJ230" t="n">
-        <v>0.9631053284160346</v>
+        <v>1.021088207590029</v>
       </c>
     </row>
     <row r="231">
@@ -28628,7 +28628,7 @@
         <v>0</v>
       </c>
       <c r="AJ231" t="n">
-        <v>1.147246590202623</v>
+        <v>1.22460440855272</v>
       </c>
     </row>
     <row r="232">
@@ -28750,7 +28750,7 @@
         <v>0</v>
       </c>
       <c r="AJ232" t="n">
-        <v>1.413336376947544</v>
+        <v>1.485127204333648</v>
       </c>
     </row>
     <row r="233">
@@ -28868,7 +28868,7 @@
         <v>0</v>
       </c>
       <c r="AJ233" t="n">
-        <v>0.8243506416577132</v>
+        <v>0.8677485536578149</v>
       </c>
     </row>
     <row r="234">
@@ -28990,7 +28990,7 @@
         <v>0</v>
       </c>
       <c r="AJ234" t="n">
-        <v>0.8962589776592632</v>
+        <v>0.938488747690586</v>
       </c>
     </row>
     <row r="235">
@@ -29112,7 +29112,7 @@
         <v>0</v>
       </c>
       <c r="AJ235" t="n">
-        <v>1.083414955312633</v>
+        <v>1.137021205962226</v>
       </c>
     </row>
     <row r="236">
@@ -29234,7 +29234,7 @@
         <v>0</v>
       </c>
       <c r="AJ236" t="n">
-        <v>0.7766986709253063</v>
+        <v>0.8198439842032866</v>
       </c>
     </row>
     <row r="237">
@@ -29356,7 +29356,7 @@
         <v>0</v>
       </c>
       <c r="AJ237" t="n">
-        <v>0.9370213318731084</v>
+        <v>0.9852854116914377</v>
       </c>
     </row>
     <row r="238">
@@ -29478,7 +29478,7 @@
         <v>0</v>
       </c>
       <c r="AJ238" t="n">
-        <v>1.118264734731881</v>
+        <v>1.118216284731881</v>
       </c>
     </row>
     <row r="239">
@@ -29600,7 +29600,7 @@
         <v>0</v>
       </c>
       <c r="AJ239" t="n">
-        <v>0.9473319609579025</v>
+        <v>0.9966120914960725</v>
       </c>
     </row>
     <row r="240">
@@ -29722,7 +29722,7 @@
         <v>0</v>
       </c>
       <c r="AJ240" t="n">
-        <v>0.6875270404433274</v>
+        <v>0.6870701404433274</v>
       </c>
     </row>
     <row r="241">
@@ -29844,7 +29844,7 @@
         <v>0</v>
       </c>
       <c r="AJ241" t="n">
-        <v>0.8987566702422297</v>
+        <v>0.8982997702422297</v>
       </c>
     </row>
     <row r="242">
@@ -29966,7 +29966,7 @@
         <v>0</v>
       </c>
       <c r="AJ242" t="n">
-        <v>0.7784886334706681</v>
+        <v>0.8218744425936478</v>
       </c>
     </row>
     <row r="243">
@@ -30084,7 +30084,7 @@
         <v>0</v>
       </c>
       <c r="AJ243" t="n">
-        <v>1.130601868154964</v>
+        <v>1.210828649473102</v>
       </c>
     </row>
     <row r="244">
@@ -30202,7 +30202,7 @@
         <v>0</v>
       </c>
       <c r="AJ244" t="n">
-        <v>0.5747879736661879</v>
+        <v>0.574376573666188</v>
       </c>
     </row>
     <row r="245">
@@ -30324,7 +30324,7 @@
         <v>0</v>
       </c>
       <c r="AJ245" t="n">
-        <v>0.8140834983168332</v>
+        <v>0.8626243199983854</v>
       </c>
     </row>
     <row r="246">
@@ -30446,7 +30446,7 @@
         <v>0</v>
       </c>
       <c r="AJ246" t="n">
-        <v>0.7744304011653483</v>
+        <v>0.8244295038502996</v>
       </c>
     </row>
     <row r="247">
@@ -30568,7 +30568,7 @@
         <v>0</v>
       </c>
       <c r="AJ247" t="n">
-        <v>0.5119490439425478</v>
+        <v>0.5119005939425478</v>
       </c>
     </row>
     <row r="248">
@@ -30686,7 +30686,7 @@
         <v>0</v>
       </c>
       <c r="AJ248" t="n">
-        <v>1.599864552961139</v>
+        <v>1.670814005289333</v>
       </c>
     </row>
     <row r="249">
@@ -30808,7 +30808,7 @@
         <v>0</v>
       </c>
       <c r="AJ249" t="n">
-        <v>0.9430104123165595</v>
+        <v>1.007226487785097</v>
       </c>
     </row>
     <row r="250">
@@ -30926,7 +30926,7 @@
         <v>0</v>
       </c>
       <c r="AJ250" t="n">
-        <v>0.5957293281006821</v>
+        <v>0.5952724281006821</v>
       </c>
     </row>
     <row r="251">
@@ -31048,7 +31048,7 @@
         <v>0</v>
       </c>
       <c r="AJ251" t="n">
-        <v>0.7410940909708237</v>
+        <v>0.7410263409708236</v>
       </c>
     </row>
     <row r="252">
@@ -31170,7 +31170,7 @@
         <v>0</v>
       </c>
       <c r="AJ252" t="n">
-        <v>0.9815786242057331</v>
+        <v>1.05910464322543</v>
       </c>
     </row>
     <row r="253">
@@ -31288,7 +31288,7 @@
         <v>0</v>
       </c>
       <c r="AJ253" t="n">
-        <v>0.9933596621466433</v>
+        <v>1.04307810846249</v>
       </c>
     </row>
     <row r="254">
@@ -31410,7 +31410,7 @@
         <v>0</v>
       </c>
       <c r="AJ254" t="n">
-        <v>1.687120161003655</v>
+        <v>1.752140308894385</v>
       </c>
     </row>
     <row r="255">
@@ -31528,7 +31528,7 @@
         <v>0</v>
       </c>
       <c r="AJ255" t="n">
-        <v>1.434999015721927</v>
+        <v>1.484482930303925</v>
       </c>
     </row>
     <row r="256">
@@ -31650,7 +31650,7 @@
         <v>0</v>
       </c>
       <c r="AJ256" t="n">
-        <v>1.492125803124199</v>
+        <v>1.55753139728274</v>
       </c>
     </row>
     <row r="257">
@@ -31772,7 +31772,7 @@
         <v>0</v>
       </c>
       <c r="AJ257" t="n">
-        <v>1.076509498850406</v>
+        <v>1.152834597631776</v>
       </c>
     </row>
     <row r="258">
@@ -31894,7 +31894,7 @@
         <v>0</v>
       </c>
       <c r="AJ258" t="n">
-        <v>0.5299027671559615</v>
+        <v>0.5298543171559615</v>
       </c>
     </row>
     <row r="259">
@@ -32016,7 +32016,7 @@
         <v>0</v>
       </c>
       <c r="AJ259" t="n">
-        <v>1.064337255752107</v>
+        <v>1.064011905752107</v>
       </c>
     </row>
     <row r="260">
@@ -32138,7 +32138,7 @@
         <v>0</v>
       </c>
       <c r="AJ260" t="n">
-        <v>1.333873291589938</v>
+        <v>1.404736149359591</v>
       </c>
     </row>
     <row r="261">
@@ -32260,7 +32260,7 @@
         <v>0</v>
       </c>
       <c r="AJ261" t="n">
-        <v>1.023138492032431</v>
+        <v>1.071890522132956</v>
       </c>
     </row>
     <row r="262">
@@ -32382,7 +32382,7 @@
         <v>0</v>
       </c>
       <c r="AJ262" t="n">
-        <v>1.003663562277961</v>
+        <v>1.070081128249043</v>
       </c>
     </row>
     <row r="263">
@@ -32500,7 +32500,7 @@
         <v>0</v>
       </c>
       <c r="AJ263" t="n">
-        <v>0.900173275056706</v>
+        <v>0.9564990595481661</v>
       </c>
     </row>
     <row r="264">
@@ -32622,7 +32622,7 @@
         <v>0</v>
       </c>
       <c r="AJ264" t="n">
-        <v>1.273885468262814</v>
+        <v>1.273417468262814</v>
       </c>
     </row>
     <row r="265">
@@ -32744,7 +32744,7 @@
         <v>0</v>
       </c>
       <c r="AJ265" t="n">
-        <v>1.521518011076922</v>
+        <v>1.583885114706084</v>
       </c>
     </row>
     <row r="266">
@@ -32866,7 +32866,7 @@
         <v>0</v>
       </c>
       <c r="AJ266" t="n">
-        <v>0.6412983623004962</v>
+        <v>0.6408414623004962</v>
       </c>
     </row>
     <row r="267">
@@ -32988,7 +32988,7 @@
         <v>0</v>
       </c>
       <c r="AJ267" t="n">
-        <v>0.7460599200474188</v>
+        <v>0.7456485200474189</v>
       </c>
     </row>
     <row r="268">
@@ -33110,7 +33110,7 @@
         <v>0</v>
       </c>
       <c r="AJ268" t="n">
-        <v>0.4446102877763364</v>
+        <v>0.4441533877763365</v>
       </c>
     </row>
     <row r="269">
@@ -33232,7 +33232,7 @@
         <v>0</v>
       </c>
       <c r="AJ269" t="n">
-        <v>0.6195444906881342</v>
+        <v>0.6195209406881342</v>
       </c>
     </row>
     <row r="270">
@@ -33350,7 +33350,7 @@
         <v>0</v>
       </c>
       <c r="AJ270" t="n">
-        <v>0.9466861168574533</v>
+        <v>1.018483709652437</v>
       </c>
     </row>
     <row r="271">
@@ -33468,7 +33468,7 @@
         <v>0</v>
       </c>
       <c r="AJ271" t="n">
-        <v>0.8226774359571865</v>
+        <v>0.8716246072191411</v>
       </c>
     </row>
     <row r="272">
@@ -33586,7 +33586,7 @@
         <v>0</v>
       </c>
       <c r="AJ272" t="n">
-        <v>0.9938372164420117</v>
+        <v>1.057492714214209</v>
       </c>
     </row>
     <row r="273">
@@ -33708,7 +33708,7 @@
         <v>0</v>
       </c>
       <c r="AJ273" t="n">
-        <v>0.8515874156465973</v>
+        <v>0.9006654482491896</v>
       </c>
     </row>
     <row r="274">
@@ -33830,7 +33830,7 @@
         <v>0</v>
       </c>
       <c r="AJ274" t="n">
-        <v>0.7034072349438983</v>
+        <v>0.7029392349438984</v>
       </c>
     </row>
     <row r="275">
@@ -33952,7 +33952,7 @@
         <v>0</v>
       </c>
       <c r="AJ275" t="n">
-        <v>1.079413123303462</v>
+        <v>1.161964092025354</v>
       </c>
     </row>
     <row r="276">
@@ -34074,7 +34074,7 @@
         <v>0</v>
       </c>
       <c r="AJ276" t="n">
-        <v>0.8899673472957079</v>
+        <v>0.9553723901705088</v>
       </c>
     </row>
     <row r="277">
@@ -34196,7 +34196,7 @@
         <v>0</v>
       </c>
       <c r="AJ277" t="n">
-        <v>1.001685410447112</v>
+        <v>1.059679289621107</v>
       </c>
     </row>
     <row r="278">
@@ -34318,7 +34318,7 @@
         <v>0</v>
       </c>
       <c r="AJ278" t="n">
-        <v>0.6421786648213056</v>
+        <v>0.6418533148213056</v>
       </c>
     </row>
     <row r="279">
@@ -34436,7 +34436,7 @@
         <v>0</v>
       </c>
       <c r="AJ279" t="n">
-        <v>0.9261887268423826</v>
+        <v>0.9942151031752935</v>
       </c>
     </row>
     <row r="280">
@@ -34558,7 +34558,7 @@
         <v>0</v>
       </c>
       <c r="AJ280" t="n">
-        <v>1.223192872257743</v>
+        <v>1.280857585305937</v>
       </c>
     </row>
     <row r="281">
@@ -34676,7 +34676,7 @@
         <v>0</v>
       </c>
       <c r="AJ281" t="n">
-        <v>0.8693488082111184</v>
+        <v>0.8693378582111183</v>
       </c>
     </row>
     <row r="282">
@@ -34798,7 +34798,7 @@
         <v>0</v>
       </c>
       <c r="AJ282" t="n">
-        <v>0.8126356490354799</v>
+        <v>0.8496260872269021</v>
       </c>
     </row>
     <row r="283">
@@ -34916,7 +34916,7 @@
         <v>0</v>
       </c>
       <c r="AJ283" t="n">
-        <v>1.268237920118261</v>
+        <v>1.334836588534</v>
       </c>
     </row>
     <row r="284">
@@ -35034,7 +35034,7 @@
         <v>0</v>
       </c>
       <c r="AJ284" t="n">
-        <v>1.227780798018956</v>
+        <v>1.276735244073863</v>
       </c>
     </row>
     <row r="285">
@@ -35156,7 +35156,7 @@
         <v>0</v>
       </c>
       <c r="AJ285" t="n">
-        <v>1.079054598022382</v>
+        <v>1.079006148022382</v>
       </c>
     </row>
     <row r="286">
@@ -35274,7 +35274,7 @@
         <v>0</v>
       </c>
       <c r="AJ286" t="n">
-        <v>0.7591222582678231</v>
+        <v>0.7968519021308089</v>
       </c>
     </row>
     <row r="287">
@@ -35396,7 +35396,7 @@
         <v>0</v>
       </c>
       <c r="AJ287" t="n">
-        <v>0.8785409159532017</v>
+        <v>0.8780729159532018</v>
       </c>
     </row>
     <row r="288">
@@ -35518,7 +35518,7 @@
         <v>0</v>
       </c>
       <c r="AJ288" t="n">
-        <v>0.9569155645261516</v>
+        <v>1.033591782807263</v>
       </c>
     </row>
     <row r="289">
@@ -35640,7 +35640,7 @@
         <v>0</v>
       </c>
       <c r="AJ289" t="n">
-        <v>1.233542977722169</v>
+        <v>1.298392716399561</v>
       </c>
     </row>
     <row r="290">
@@ -35762,7 +35762,7 @@
         <v>0</v>
       </c>
       <c r="AJ290" t="n">
-        <v>1.097985601353492</v>
+        <v>1.097517601353492</v>
       </c>
     </row>
     <row r="291">
@@ -35884,7 +35884,7 @@
         <v>0</v>
       </c>
       <c r="AJ291" t="n">
-        <v>1.009109995384206</v>
+        <v>1.066876368751342</v>
       </c>
     </row>
     <row r="292">
@@ -36006,7 +36006,7 @@
         <v>0</v>
       </c>
       <c r="AJ292" t="n">
-        <v>0.5187203787327901</v>
+        <v>0.5185872287327902</v>
       </c>
     </row>
     <row r="293">
@@ -36128,7 +36128,7 @@
         <v>0</v>
       </c>
       <c r="AJ293" t="n">
-        <v>0.838962936660828</v>
+        <v>0.8872168782323948</v>
       </c>
     </row>
     <row r="294">
@@ -36250,7 +36250,7 @@
         <v>0</v>
       </c>
       <c r="AJ294" t="n">
-        <v>0.9822604088174376</v>
+        <v>1.053457501562895</v>
       </c>
     </row>
     <row r="295">
@@ -36368,7 +36368,7 @@
         <v>0</v>
       </c>
       <c r="AJ295" t="n">
-        <v>1.176907099126035</v>
+        <v>1.258627330048444</v>
       </c>
     </row>
     <row r="296">
@@ -36490,7 +36490,7 @@
         <v>0</v>
       </c>
       <c r="AJ296" t="n">
-        <v>1.212724175974983</v>
+        <v>1.261645824235798</v>
       </c>
     </row>
     <row r="297">
@@ -36612,7 +36612,7 @@
         <v>0</v>
       </c>
       <c r="AJ297" t="n">
-        <v>1.018241488006685</v>
+        <v>1.017773488006684</v>
       </c>
     </row>
     <row r="298">
@@ -36734,7 +36734,7 @@
         <v>0</v>
       </c>
       <c r="AJ298" t="n">
-        <v>0.8286164229583739</v>
+        <v>0.8914445648251489</v>
       </c>
     </row>
     <row r="299">
@@ -36852,7 +36852,7 @@
         <v>0</v>
       </c>
       <c r="AJ299" t="n">
-        <v>0.7144020821928699</v>
+        <v>0.7143846321928699</v>
       </c>
     </row>
     <row r="300">
@@ -36975,7 +36975,7 @@
         <v>0</v>
       </c>
       <c r="AJ300" t="n">
-        <v>0.5008687967271196</v>
+        <v>0.5008576967271197</v>
       </c>
     </row>
     <row r="301">
@@ -37093,7 +37093,7 @@
         <v>0</v>
       </c>
       <c r="AJ301" t="n">
-        <v>0.9418019802171913</v>
+        <v>1.01157591346994</v>
       </c>
     </row>
     <row r="302">
@@ -37211,7 +37211,7 @@
         <v>0</v>
       </c>
       <c r="AJ302" t="n">
-        <v>1.14894381755586</v>
+        <v>1.214338162982603</v>
       </c>
     </row>
     <row r="303">
@@ -37333,7 +37333,7 @@
         <v>0</v>
       </c>
       <c r="AJ303" t="n">
-        <v>1.413378338043118</v>
+        <v>1.477294849657589</v>
       </c>
     </row>
     <row r="304">
@@ -37451,7 +37451,7 @@
         <v>0</v>
       </c>
       <c r="AJ304" t="n">
-        <v>1.078347094344755</v>
+        <v>1.127708571159135</v>
       </c>
     </row>
     <row r="305">
@@ -37569,7 +37569,7 @@
         <v>0</v>
       </c>
       <c r="AJ305" t="n">
-        <v>0.8789105605447606</v>
+        <v>0.9428329670994249</v>
       </c>
     </row>
     <row r="306">
@@ -37687,7 +37687,7 @@
         <v>0</v>
       </c>
       <c r="AJ306" t="n">
-        <v>1.267993890238433</v>
+        <v>1.32447086792025</v>
       </c>
     </row>
     <row r="307">
@@ -37809,7 +37809,7 @@
         <v>0</v>
       </c>
       <c r="AJ307" t="n">
-        <v>0.9444306355664803</v>
+        <v>1.008591158450882</v>
       </c>
     </row>
     <row r="308">
@@ -37927,7 +37927,7 @@
         <v>0</v>
       </c>
       <c r="AJ308" t="n">
-        <v>0.8708424562568096</v>
+        <v>0.9170124839134677</v>
       </c>
     </row>
     <row r="309">
@@ -38045,7 +38045,7 @@
         <v>0</v>
       </c>
       <c r="AJ309" t="n">
-        <v>0.8984977692683598</v>
+        <v>0.9490745788363608</v>
       </c>
     </row>
     <row r="310">
@@ -38167,7 +38167,7 @@
         <v>0</v>
       </c>
       <c r="AJ310" t="n">
-        <v>0.880145822909579</v>
+        <v>0.9449413847288219</v>
       </c>
     </row>
     <row r="311">
@@ -38285,7 +38285,7 @@
         <v>0</v>
       </c>
       <c r="AJ311" t="n">
-        <v>0.7713418512483221</v>
+        <v>0.8205475564383908</v>
       </c>
     </row>
     <row r="312">
@@ -38403,7 +38403,7 @@
         <v>0</v>
       </c>
       <c r="AJ312" t="n">
-        <v>0.8502876611786617</v>
+        <v>0.8991810550625478</v>
       </c>
     </row>
     <row r="313">
@@ -38521,7 +38521,7 @@
         <v>0</v>
       </c>
       <c r="AJ313" t="n">
-        <v>0.823694346241276</v>
+        <v>0.871757027913926</v>
       </c>
     </row>
     <row r="314">
@@ -38643,7 +38643,7 @@
         <v>0</v>
       </c>
       <c r="AJ314" t="n">
-        <v>1.081873880514575</v>
+        <v>1.137774595380197</v>
       </c>
     </row>
     <row r="315">
@@ -38761,7 +38761,7 @@
         <v>0</v>
       </c>
       <c r="AJ315" t="n">
-        <v>0.739372080854779</v>
+        <v>0.7729946975219504</v>
       </c>
     </row>
     <row r="316">
@@ -38883,7 +38883,7 @@
         <v>0</v>
       </c>
       <c r="AJ316" t="n">
-        <v>0.9607568189515661</v>
+        <v>1.026775150073478</v>
       </c>
     </row>
     <row r="317">
@@ -39001,7 +39001,7 @@
         <v>0</v>
       </c>
       <c r="AJ317" t="n">
-        <v>0.6175730793556041</v>
+        <v>0.6379368557120759</v>
       </c>
     </row>
     <row r="318">
@@ -39123,7 +39123,7 @@
         <v>0</v>
       </c>
       <c r="AJ318" t="n">
-        <v>1.082641109140838</v>
+        <v>1.154543975337686</v>
       </c>
     </row>
     <row r="319">
@@ -39241,7 +39241,7 @@
         <v>0</v>
       </c>
       <c r="AJ319" t="n">
-        <v>1.032823688598224</v>
+        <v>1.103417198023252</v>
       </c>
     </row>
     <row r="320">
@@ -39363,7 +39363,7 @@
         <v>0</v>
       </c>
       <c r="AJ320" t="n">
-        <v>1.150185403005038</v>
+        <v>1.230408016124561</v>
       </c>
     </row>
     <row r="321">
@@ -39481,7 +39481,7 @@
         <v>0</v>
       </c>
       <c r="AJ321" t="n">
-        <v>0.8393454782533019</v>
+        <v>0.8973524644400391</v>
       </c>
     </row>
     <row r="322">
@@ -39599,7 +39599,7 @@
         <v>0</v>
       </c>
       <c r="AJ322" t="n">
-        <v>0.9642429937390659</v>
+        <v>1.032992015777296</v>
       </c>
     </row>
     <row r="323">
@@ -39721,7 +39721,7 @@
         <v>0</v>
       </c>
       <c r="AJ323" t="n">
-        <v>0.8395178193392769</v>
+        <v>0.8937173703197223</v>
       </c>
     </row>
     <row r="324">
@@ -39839,7 +39839,7 @@
         <v>0</v>
       </c>
       <c r="AJ324" t="n">
-        <v>1.093651500466969</v>
+        <v>1.142179999213882</v>
       </c>
     </row>
     <row r="325">
@@ -39961,7 +39961,7 @@
         <v>0</v>
       </c>
       <c r="AJ325" t="n">
-        <v>0.8955806184712046</v>
+        <v>0.9511631668430977</v>
       </c>
     </row>
     <row r="326">
@@ -40079,7 +40079,7 @@
         <v>0</v>
       </c>
       <c r="AJ326" t="n">
-        <v>1.112015252607956</v>
+        <v>1.176378407280026</v>
       </c>
     </row>
     <row r="327">
@@ -40197,7 +40197,7 @@
         <v>0</v>
       </c>
       <c r="AJ327" t="n">
-        <v>0.7472004050413645</v>
+        <v>0.8199408022148571</v>
       </c>
     </row>
     <row r="328">
@@ -40319,7 +40319,7 @@
         <v>0</v>
       </c>
       <c r="AJ328" t="n">
-        <v>0.928409832320912</v>
+        <v>0.9995772510981604</v>
       </c>
     </row>
     <row r="329">
@@ -40441,7 +40441,7 @@
         <v>0</v>
       </c>
       <c r="AJ329" t="n">
-        <v>0.8499534454839426</v>
+        <v>0.897500106027917</v>
       </c>
     </row>
     <row r="330">
@@ -40563,7 +40563,7 @@
         <v>0</v>
       </c>
       <c r="AJ330" t="n">
-        <v>1.058042386393292</v>
+        <v>1.124043764620542</v>
       </c>
     </row>
     <row r="331">
@@ -40685,7 +40685,7 @@
         <v>0</v>
       </c>
       <c r="AJ331" t="n">
-        <v>0.8495273085920082</v>
+        <v>0.8494890585920082</v>
       </c>
     </row>
     <row r="332">
@@ -40807,7 +40807,7 @@
         <v>0</v>
       </c>
       <c r="AJ332" t="n">
-        <v>1.38363909346004</v>
+        <v>1.463036674509546</v>
       </c>
     </row>
     <row r="333">
@@ -40925,7 +40925,7 @@
         <v>0</v>
       </c>
       <c r="AJ333" t="n">
-        <v>1.116450238148548</v>
+        <v>1.171157574796366</v>
       </c>
     </row>
     <row r="334">
@@ -41043,7 +41043,7 @@
         <v>0</v>
       </c>
       <c r="AJ334" t="n">
-        <v>1.020511949222177</v>
+        <v>1.081986820794462</v>
       </c>
     </row>
     <row r="335">
@@ -41165,7 +41165,7 @@
         <v>0</v>
       </c>
       <c r="AJ335" t="n">
-        <v>0.7033312235573469</v>
+        <v>0.703240823557347</v>
       </c>
     </row>
     <row r="336">
@@ -41283,7 +41283,7 @@
         <v>0</v>
       </c>
       <c r="AJ336" t="n">
-        <v>0.8603441421436897</v>
+        <v>0.9237221094625508</v>
       </c>
     </row>
     <row r="337">
@@ -41405,7 +41405,7 @@
         <v>0</v>
       </c>
       <c r="AJ337" t="n">
-        <v>1.463653709989406</v>
+        <v>1.527889104878332</v>
       </c>
     </row>
     <row r="338">
@@ -41523,7 +41523,7 @@
         <v>0</v>
       </c>
       <c r="AJ338" t="n">
-        <v>1.270739109829784</v>
+        <v>1.327158390976689</v>
       </c>
     </row>
     <row r="339">
@@ -41641,7 +41641,7 @@
         <v>0</v>
       </c>
       <c r="AJ339" t="n">
-        <v>0.8318607894846545</v>
+        <v>0.8841658429246106</v>
       </c>
     </row>
     <row r="340">
@@ -41763,7 +41763,7 @@
         <v>0</v>
       </c>
       <c r="AJ340" t="n">
-        <v>1.008602430039037</v>
+        <v>1.060906233478993</v>
       </c>
     </row>
     <row r="341">
@@ -41881,7 +41881,7 @@
         <v>0</v>
       </c>
       <c r="AJ341" t="n">
-        <v>1.279955137380269</v>
+        <v>1.34597401850218</v>
       </c>
     </row>
     <row r="342">
@@ -42003,7 +42003,7 @@
         <v>0</v>
       </c>
       <c r="AJ342" t="n">
-        <v>1.218789311926684</v>
+        <v>1.282275062944348</v>
       </c>
     </row>
     <row r="343">
@@ -42125,7 +42125,7 @@
         <v>0</v>
       </c>
       <c r="AJ343" t="n">
-        <v>1.020573901994436</v>
+        <v>1.077135880559634</v>
       </c>
     </row>
     <row r="344">
@@ -42247,7 +42247,7 @@
         <v>0</v>
       </c>
       <c r="AJ344" t="n">
-        <v>1.338470822460585</v>
+        <v>1.398459569953176</v>
       </c>
     </row>
     <row r="345">
@@ -42365,7 +42365,7 @@
         <v>0</v>
       </c>
       <c r="AJ345" t="n">
-        <v>0.7855945480259114</v>
+        <v>0.8470456484249165</v>
       </c>
     </row>
     <row r="346">
@@ -42487,7 +42487,7 @@
         <v>0</v>
       </c>
       <c r="AJ346" t="n">
-        <v>0.9902801912287519</v>
+        <v>1.052514408312166</v>
       </c>
     </row>
     <row r="347">
@@ -42609,7 +42609,7 @@
         <v>0</v>
       </c>
       <c r="AJ347" t="n">
-        <v>1.069618573470497</v>
+        <v>1.131141622096895</v>
       </c>
     </row>
     <row r="348">
@@ -42731,7 +42731,7 @@
         <v>0</v>
       </c>
       <c r="AJ348" t="n">
-        <v>1.133868441756728</v>
+        <v>1.193444131486028</v>
       </c>
     </row>
     <row r="349">
@@ -42853,7 +42853,7 @@
         <v>0</v>
       </c>
       <c r="AJ349" t="n">
-        <v>1.227921202536894</v>
+        <v>1.299406735033347</v>
       </c>
     </row>
     <row r="350">
@@ -42971,7 +42971,7 @@
         <v>0</v>
       </c>
       <c r="AJ350" t="n">
-        <v>0.9884216365990686</v>
+        <v>1.05418819431277</v>
       </c>
     </row>
     <row r="351">
@@ -43089,7 +43089,7 @@
         <v>0</v>
       </c>
       <c r="AJ351" t="n">
-        <v>0.8556708285583917</v>
+        <v>0.9045795386334662</v>
       </c>
     </row>
     <row r="352">
@@ -43211,7 +43211,7 @@
         <v>0</v>
       </c>
       <c r="AJ352" t="n">
-        <v>0.9849508575611805</v>
+        <v>1.048940366356069</v>
       </c>
     </row>
     <row r="353">
@@ -43333,7 +43333,7 @@
         <v>0</v>
       </c>
       <c r="AJ353" t="n">
-        <v>0.6231681602105393</v>
+        <v>0.6231376102105394</v>
       </c>
     </row>
     <row r="354">
@@ -43451,7 +43451,7 @@
         <v>0</v>
       </c>
       <c r="AJ354" t="n">
-        <v>1.027931408370238</v>
+        <v>1.075291376355997</v>
       </c>
     </row>
     <row r="355">
@@ -43573,7 +43573,7 @@
         <v>0</v>
       </c>
       <c r="AJ355" t="n">
-        <v>0.5561320912664756</v>
+        <v>0.5561205412664756</v>
       </c>
     </row>
     <row r="356">
@@ -43695,7 +43695,7 @@
         <v>0</v>
       </c>
       <c r="AJ356" t="n">
-        <v>1.107666718066685</v>
+        <v>1.165488191789052</v>
       </c>
     </row>
     <row r="357">
@@ -43817,7 +43817,7 @@
         <v>0</v>
       </c>
       <c r="AJ357" t="n">
-        <v>0.8423358529802649</v>
+        <v>0.8905901205446917</v>
       </c>
     </row>
     <row r="358">
@@ -43935,7 +43935,7 @@
         <v>0</v>
       </c>
       <c r="AJ358" t="n">
-        <v>1.321983730038472</v>
+        <v>1.379075510428788</v>
       </c>
     </row>
     <row r="359">
@@ -44057,7 +44057,7 @@
         <v>0</v>
       </c>
       <c r="AJ359" t="n">
-        <v>0.8725622681637086</v>
+        <v>0.9215947321849139</v>
       </c>
     </row>
     <row r="360">
@@ -44179,7 +44179,7 @@
         <v>0</v>
       </c>
       <c r="AJ360" t="n">
-        <v>1.897597083699902</v>
+        <v>1.969545964764595</v>
       </c>
     </row>
     <row r="361">
@@ -44301,7 +44301,7 @@
         <v>0</v>
       </c>
       <c r="AJ361" t="n">
-        <v>1.539026600108451</v>
+        <v>1.597551554389408</v>
       </c>
     </row>
     <row r="362">
@@ -44419,7 +44419,7 @@
         <v>0</v>
       </c>
       <c r="AJ362" t="n">
-        <v>0.8669491153342194</v>
+        <v>0.9232748998256796</v>
       </c>
     </row>
     <row r="363">
@@ -44541,7 +44541,7 @@
         <v>0</v>
       </c>
       <c r="AJ363" t="n">
-        <v>0.9499649590226661</v>
+        <v>1.012432006260436</v>
       </c>
     </row>
     <row r="364">
@@ -44663,7 +44663,7 @@
         <v>0</v>
       </c>
       <c r="AJ364" t="n">
-        <v>1.084204348080548</v>
+        <v>1.164768709137029</v>
       </c>
     </row>
     <row r="365">
@@ -44785,7 +44785,7 @@
         <v>0</v>
       </c>
       <c r="AJ365" t="n">
-        <v>0.9744225723636779</v>
+        <v>1.030015139472722</v>
       </c>
     </row>
     <row r="366">
@@ -44907,7 +44907,7 @@
         <v>0</v>
       </c>
       <c r="AJ366" t="n">
-        <v>0.8105954914696891</v>
+        <v>0.8617900020651388</v>
       </c>
     </row>
     <row r="367">
@@ -45025,7 +45025,7 @@
         <v>0</v>
       </c>
       <c r="AJ367" t="n">
-        <v>0.8217254640891911</v>
+        <v>0.8700725000497508</v>
       </c>
     </row>
     <row r="368">
@@ -45143,7 +45143,7 @@
         <v>0</v>
       </c>
       <c r="AJ368" t="n">
-        <v>0.9968713890922354</v>
+        <v>1.045742553809369</v>
       </c>
     </row>
     <row r="369">
@@ -45261,7 +45261,7 @@
         <v>0</v>
       </c>
       <c r="AJ369" t="n">
-        <v>1.098102078141459</v>
+        <v>1.118791091281928</v>
       </c>
     </row>
     <row r="370">
@@ -45383,7 +45383,7 @@
         <v>0</v>
       </c>
       <c r="AJ370" t="n">
-        <v>0.597221818241942</v>
+        <v>0.5971296682419419</v>
       </c>
     </row>
     <row r="371">
@@ -45505,7 +45505,7 @@
         <v>0</v>
       </c>
       <c r="AJ371" t="n">
-        <v>0.9204010296765768</v>
+        <v>0.9787998080303336</v>
       </c>
     </row>
     <row r="372">
@@ -45627,7 +45627,7 @@
         <v>0</v>
       </c>
       <c r="AJ372" t="n">
-        <v>0.8787384630583309</v>
+        <v>0.9372363418753887</v>
       </c>
     </row>
     <row r="373">
@@ -45745,7 +45745,7 @@
         <v>0</v>
       </c>
       <c r="AJ373" t="n">
-        <v>1.037444840784388</v>
+        <v>1.1268634064606</v>
       </c>
     </row>
     <row r="374">
@@ -45867,7 +45867,7 @@
         <v>0</v>
       </c>
       <c r="AJ374" t="n">
-        <v>0.4934804400469028</v>
+        <v>0.4934557400469028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hopkins statistic test for clustering and opt improvement
</commit_message>
<xml_diff>
--- a/src/results/data_deliq_scores.xlsx
+++ b/src/results/data_deliq_scores.xlsx
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.7925373904460953</v>
+        <v>1.002870838214557</v>
       </c>
     </row>
     <row r="3">
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.9923836931244895</v>
+        <v>0.9759286601758963</v>
       </c>
     </row>
     <row r="4">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0.9538685792706206</v>
+        <v>1.332534829861843</v>
       </c>
     </row>
     <row r="5">
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0.8476201109767462</v>
+        <v>0.02422178031362132</v>
       </c>
     </row>
     <row r="6">
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.9766291175100404</v>
+        <v>1.250191173731501</v>
       </c>
     </row>
     <row r="7">
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.8527870111403643</v>
+        <v>0.8617108638139451</v>
       </c>
     </row>
     <row r="8">
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.5744743178143384</v>
+        <v>0.01641520479469538</v>
       </c>
     </row>
     <row r="9">
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.5537217427313912</v>
+        <v>0.01583216407803975</v>
       </c>
     </row>
     <row r="10">
@@ -1702,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0.4934422400469028</v>
+        <v>0.01409899114419722</v>
       </c>
     </row>
     <row r="11">
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" t="n">
-        <v>0.9694074318081948</v>
+        <v>1.12063247575742</v>
       </c>
     </row>
     <row r="12">
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" t="n">
-        <v>1.692604419621658</v>
+        <v>1.10376479628293</v>
       </c>
     </row>
     <row r="13">
@@ -2068,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="AJ13" t="n">
-        <v>0.9721752402978235</v>
+        <v>1.349260289747418</v>
       </c>
     </row>
     <row r="14">
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="AJ14" t="n">
-        <v>0.8841043657503401</v>
+        <v>0.02526418759286687</v>
       </c>
     </row>
     <row r="15">
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="AJ15" t="n">
-        <v>1.498358306430684</v>
+        <v>1.136803614429223</v>
       </c>
     </row>
     <row r="16">
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="AJ16" t="n">
-        <v>0.457982052776905</v>
+        <v>0.01310914579362586</v>
       </c>
     </row>
     <row r="17">
@@ -2552,7 +2552,7 @@
         <v>0</v>
       </c>
       <c r="AJ17" t="n">
-        <v>0.5737116851717258</v>
+        <v>0.01639296671919217</v>
       </c>
     </row>
     <row r="18">
@@ -2674,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="AJ18" t="n">
-        <v>0.6402567148213055</v>
+        <v>0.01829474185203731</v>
       </c>
     </row>
     <row r="19">
@@ -2796,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="AJ19" t="n">
-        <v>0.6878076054200574</v>
+        <v>0.01965500301200164</v>
       </c>
     </row>
     <row r="20">
@@ -2918,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="AJ20" t="n">
-        <v>1.122050436715656</v>
+        <v>1.296098124319623</v>
       </c>
     </row>
     <row r="21">
@@ -3040,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="AJ21" t="n">
-        <v>0.7940115170779454</v>
+        <v>0.8301061812206405</v>
       </c>
     </row>
     <row r="22">
@@ -3162,7 +3162,7 @@
         <v>0</v>
       </c>
       <c r="AJ22" t="n">
-        <v>0.4749351389380377</v>
+        <v>0.01357384254108679</v>
       </c>
     </row>
     <row r="23">
@@ -3284,7 +3284,7 @@
         <v>0</v>
       </c>
       <c r="AJ23" t="n">
-        <v>0.4877589449107392</v>
+        <v>0.01393759556887826</v>
       </c>
     </row>
     <row r="24">
@@ -3406,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="AJ24" t="n">
-        <v>0.724129597861573</v>
+        <v>0.0206900456531878</v>
       </c>
     </row>
     <row r="25">
@@ -3528,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" t="n">
-        <v>0.5709366053160996</v>
+        <v>0.01631292586617427</v>
       </c>
     </row>
     <row r="26">
@@ -3650,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" t="n">
-        <v>1.463705891459361</v>
+        <v>0.8796296618603757</v>
       </c>
     </row>
     <row r="27">
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="AJ27" t="n">
-        <v>0.8144935214615044</v>
+        <v>1.198943348984672</v>
       </c>
     </row>
     <row r="28">
@@ -3894,7 +3894,7 @@
         <v>0</v>
       </c>
       <c r="AJ28" t="n">
-        <v>0.8119003835806357</v>
+        <v>0.02319785381658959</v>
       </c>
     </row>
     <row r="29">
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="AJ29" t="n">
-        <v>1.159270868958391</v>
+        <v>1.371742522863116</v>
       </c>
     </row>
     <row r="30">
@@ -4138,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="AJ30" t="n">
-        <v>0.8598697457202481</v>
+        <v>1.091731499433917</v>
       </c>
     </row>
     <row r="31">
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="AJ31" t="n">
-        <v>1.029680316774951</v>
+        <v>1.090970622119106</v>
       </c>
     </row>
     <row r="32">
@@ -4382,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="AJ32" t="n">
-        <v>0.6959912237283377</v>
+        <v>0.5580367126527569</v>
       </c>
     </row>
     <row r="33">
@@ -4504,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="AJ33" t="n">
-        <v>0.518453206953802</v>
+        <v>0.01481542019868006</v>
       </c>
     </row>
     <row r="34">
@@ -4626,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" t="n">
-        <v>0.9520116205626161</v>
+        <v>1.225540785691208</v>
       </c>
     </row>
     <row r="35">
@@ -4748,7 +4748,7 @@
         <v>0</v>
       </c>
       <c r="AJ35" t="n">
-        <v>0.9658244922144728</v>
+        <v>1.330532825114035</v>
       </c>
     </row>
     <row r="36">
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
       <c r="AJ36" t="n">
-        <v>1.016288806548552</v>
+        <v>1.074935658958299</v>
       </c>
     </row>
     <row r="37">
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="AJ37" t="n">
-        <v>0.6389225885395416</v>
+        <v>0.01825553395827262</v>
       </c>
     </row>
     <row r="38">
@@ -5114,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="AJ38" t="n">
-        <v>0.8886252607326957</v>
+        <v>0.02539335602093416</v>
       </c>
     </row>
     <row r="39">
@@ -5236,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="AJ39" t="n">
-        <v>0.9566470729316165</v>
+        <v>1.095307510530436</v>
       </c>
     </row>
     <row r="40">
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" t="n">
-        <v>0.7306776590109646</v>
+        <v>0.02088126168602756</v>
       </c>
     </row>
     <row r="41">
@@ -5480,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.6846489416075733</v>
+        <v>0.01956206976021638</v>
       </c>
     </row>
     <row r="42">
@@ -5602,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="AJ42" t="n">
-        <v>1.049748373761341</v>
+        <v>1.67863690588144</v>
       </c>
     </row>
     <row r="43">
@@ -5724,7 +5724,7 @@
         <v>0</v>
       </c>
       <c r="AJ43" t="n">
-        <v>1.016478704912432</v>
+        <v>1.421583982570792</v>
       </c>
     </row>
     <row r="44">
@@ -5842,7 +5842,7 @@
         <v>0</v>
       </c>
       <c r="AJ44" t="n">
-        <v>0.4934920812763994</v>
+        <v>0.01410404089361141</v>
       </c>
     </row>
     <row r="45">
@@ -5964,7 +5964,7 @@
         <v>0</v>
       </c>
       <c r="AJ45" t="n">
-        <v>1.044996899998732</v>
+        <v>1.204368794163151</v>
       </c>
     </row>
     <row r="46">
@@ -6086,7 +6086,7 @@
         <v>0</v>
       </c>
       <c r="AJ46" t="n">
-        <v>1.183982259576716</v>
+        <v>1.415729001642433</v>
       </c>
     </row>
     <row r="47">
@@ -6208,7 +6208,7 @@
         <v>0</v>
       </c>
       <c r="AJ47" t="n">
-        <v>0.664280482200032</v>
+        <v>0.01900038949142949</v>
       </c>
     </row>
     <row r="48">
@@ -6330,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" t="n">
-        <v>1.578028125533047</v>
+        <v>1.113719239109364</v>
       </c>
     </row>
     <row r="49">
@@ -6452,7 +6452,7 @@
         <v>0</v>
       </c>
       <c r="AJ49" t="n">
-        <v>0.6534586279425454</v>
+        <v>0.01867512079835844</v>
       </c>
     </row>
     <row r="50">
@@ -6574,7 +6574,7 @@
         <v>0</v>
       </c>
       <c r="AJ50" t="n">
-        <v>0.4934545400469028</v>
+        <v>0.01409940114419722</v>
       </c>
     </row>
     <row r="51">
@@ -6696,7 +6696,7 @@
         <v>0</v>
       </c>
       <c r="AJ51" t="n">
-        <v>0.8693633448586154</v>
+        <v>0.9664704927287587</v>
       </c>
     </row>
     <row r="52">
@@ -6818,7 +6818,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" t="n">
-        <v>0.5784870851717258</v>
+        <v>0.01655214671919216</v>
       </c>
     </row>
     <row r="53">
@@ -6940,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="AJ53" t="n">
-        <v>0.7548198096938955</v>
+        <v>0.6831248777574033</v>
       </c>
     </row>
     <row r="54">
@@ -7062,7 +7062,7 @@
         <v>0</v>
       </c>
       <c r="AJ54" t="n">
-        <v>0.4608973871216572</v>
+        <v>0.01316960106061878</v>
       </c>
     </row>
     <row r="55">
@@ -7184,7 +7184,7 @@
         <v>0</v>
       </c>
       <c r="AJ55" t="n">
-        <v>0.4741086389380377</v>
+        <v>0.01354629254108679</v>
       </c>
     </row>
     <row r="56">
@@ -7306,7 +7306,7 @@
         <v>0</v>
       </c>
       <c r="AJ56" t="n">
-        <v>0.4953603712167742</v>
+        <v>0.01415375632047926</v>
       </c>
     </row>
     <row r="57">
@@ -7428,7 +7428,7 @@
         <v>0</v>
       </c>
       <c r="AJ57" t="n">
-        <v>0.5491441594943232</v>
+        <v>0.01569470741412352</v>
       </c>
     </row>
     <row r="58">
@@ -7550,7 +7550,7 @@
         <v>0</v>
       </c>
       <c r="AJ58" t="n">
-        <v>1.209228534529375</v>
+        <v>1.419727174739448</v>
       </c>
     </row>
     <row r="59">
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
       <c r="AJ59" t="n">
-        <v>0.9062517520653459</v>
+        <v>0.02589697005900989</v>
       </c>
     </row>
     <row r="60">
@@ -7794,7 +7794,7 @@
         <v>0</v>
       </c>
       <c r="AJ60" t="n">
-        <v>1.154179464354207</v>
+        <v>1.360529356448463</v>
       </c>
     </row>
     <row r="61">
@@ -7916,7 +7916,7 @@
         <v>0</v>
       </c>
       <c r="AJ61" t="n">
-        <v>0.8334780990825774</v>
+        <v>0.8658855645558522</v>
       </c>
     </row>
     <row r="62">
@@ -8038,7 +8038,7 @@
         <v>0</v>
       </c>
       <c r="AJ62" t="n">
-        <v>0.683434910437702</v>
+        <v>0.01953077458393435</v>
       </c>
     </row>
     <row r="63">
@@ -8160,7 +8160,7 @@
         <v>0</v>
       </c>
       <c r="AJ63" t="n">
-        <v>0.877721102204935</v>
+        <v>0.9650553613747294</v>
       </c>
     </row>
     <row r="64">
@@ -8278,7 +8278,7 @@
         <v>0</v>
       </c>
       <c r="AJ64" t="n">
-        <v>0.4772505538857703</v>
+        <v>0.01365967439673629</v>
       </c>
     </row>
     <row r="65">
@@ -8400,7 +8400,7 @@
         <v>0</v>
       </c>
       <c r="AJ65" t="n">
-        <v>0.9330837875189633</v>
+        <v>0.02666289392911324</v>
       </c>
     </row>
     <row r="66">
@@ -8522,7 +8522,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" t="n">
-        <v>1.032685685891819</v>
+        <v>1.399824224108612</v>
       </c>
     </row>
     <row r="67">
@@ -8644,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="AJ67" t="n">
-        <v>0.5284608425480435</v>
+        <v>0.01510314835851553</v>
       </c>
     </row>
     <row r="68">
@@ -8766,7 +8766,7 @@
         <v>0</v>
       </c>
       <c r="AJ68" t="n">
-        <v>0.529637973717915</v>
+        <v>0.01513321353479757</v>
       </c>
     </row>
     <row r="69">
@@ -8888,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="AJ69" t="n">
-        <v>0.9625011009970907</v>
+        <v>1.048652253913699</v>
       </c>
     </row>
     <row r="70">
@@ -9010,7 +9010,7 @@
         <v>0</v>
       </c>
       <c r="AJ70" t="n">
-        <v>0.8302894943463935</v>
+        <v>0.02372325698132553</v>
       </c>
     </row>
     <row r="71">
@@ -9132,7 +9132,7 @@
         <v>0</v>
       </c>
       <c r="AJ71" t="n">
-        <v>0.6131422414257253</v>
+        <v>0.01751927261216358</v>
       </c>
     </row>
     <row r="72">
@@ -9254,7 +9254,7 @@
         <v>0</v>
       </c>
       <c r="AJ72" t="n">
-        <v>0.5545317426795556</v>
+        <v>0.01584852121941588</v>
       </c>
     </row>
     <row r="73">
@@ -9376,7 +9376,7 @@
         <v>0</v>
       </c>
       <c r="AJ73" t="n">
-        <v>0.5284608425480435</v>
+        <v>0.01510314835851553</v>
       </c>
     </row>
     <row r="74">
@@ -9498,7 +9498,7 @@
         <v>0</v>
       </c>
       <c r="AJ74" t="n">
-        <v>0.6710780939095223</v>
+        <v>0.01918541411170064</v>
       </c>
     </row>
     <row r="75">
@@ -9620,7 +9620,7 @@
         <v>0</v>
       </c>
       <c r="AJ75" t="n">
-        <v>0.5787770304493395</v>
+        <v>0.0165381794414097</v>
       </c>
     </row>
     <row r="76">
@@ -9742,7 +9742,7 @@
         <v>0</v>
       </c>
       <c r="AJ76" t="n">
-        <v>0.9119019879321669</v>
+        <v>1.090868965434061</v>
       </c>
     </row>
     <row r="77">
@@ -9865,7 +9865,7 @@
         <v>0</v>
       </c>
       <c r="AJ77" t="n">
-        <v>0.9413200973498507</v>
+        <v>0.9715551035167717</v>
       </c>
     </row>
     <row r="78">
@@ -9987,7 +9987,7 @@
         <v>0</v>
       </c>
       <c r="AJ78" t="n">
-        <v>1.136532742823891</v>
+        <v>1.507000474276814</v>
       </c>
     </row>
     <row r="79">
@@ -10109,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="AJ79" t="n">
-        <v>0.687610010437702</v>
+        <v>0.01966994458393434</v>
       </c>
     </row>
     <row r="80">
@@ -10231,7 +10231,7 @@
         <v>0</v>
       </c>
       <c r="AJ80" t="n">
-        <v>1.023357029158501</v>
+        <v>1.277234520152132</v>
       </c>
     </row>
     <row r="81">
@@ -10353,7 +10353,7 @@
         <v>0</v>
       </c>
       <c r="AJ81" t="n">
-        <v>0.8510445695975998</v>
+        <v>1.067984178387861</v>
       </c>
     </row>
     <row r="82">
@@ -10475,7 +10475,7 @@
         <v>0</v>
       </c>
       <c r="AJ82" t="n">
-        <v>0.5774060490524714</v>
+        <v>0.01649864997292776</v>
       </c>
     </row>
     <row r="83">
@@ -10597,7 +10597,7 @@
         <v>0</v>
       </c>
       <c r="AJ83" t="n">
-        <v>0.9813529252973711</v>
+        <v>0.4176875039726861</v>
       </c>
     </row>
     <row r="84">
@@ -10719,7 +10719,7 @@
         <v>0</v>
       </c>
       <c r="AJ84" t="n">
-        <v>0.9190961582035315</v>
+        <v>1.075900740921848</v>
       </c>
     </row>
     <row r="85">
@@ -10841,7 +10841,7 @@
         <v>0</v>
       </c>
       <c r="AJ85" t="n">
-        <v>1.363273829147948</v>
+        <v>1.25853898994796</v>
       </c>
     </row>
     <row r="86">
@@ -10963,7 +10963,7 @@
         <v>0</v>
       </c>
       <c r="AJ86" t="n">
-        <v>1.552148596586929</v>
+        <v>1.351829722812123</v>
       </c>
     </row>
     <row r="87">
@@ -11085,7 +11085,7 @@
         <v>0</v>
       </c>
       <c r="AJ87" t="n">
-        <v>0.695439362100274</v>
+        <v>0.01987375891715069</v>
       </c>
     </row>
     <row r="88">
@@ -11207,7 +11207,7 @@
         <v>0</v>
       </c>
       <c r="AJ88" t="n">
-        <v>0.9614527671914875</v>
+        <v>0.8648159439868344</v>
       </c>
     </row>
     <row r="89">
@@ -11329,7 +11329,7 @@
         <v>0</v>
       </c>
       <c r="AJ89" t="n">
-        <v>0.4934422400469028</v>
+        <v>0.01409899114419722</v>
       </c>
     </row>
     <row r="90">
@@ -11451,7 +11451,7 @@
         <v>0</v>
       </c>
       <c r="AJ90" t="n">
-        <v>0.9456944767608589</v>
+        <v>1.271447947949253</v>
       </c>
     </row>
     <row r="91">
@@ -11573,7 +11573,7 @@
         <v>0</v>
       </c>
       <c r="AJ91" t="n">
-        <v>0.4643496416967175</v>
+        <v>0.01326777404847764</v>
       </c>
     </row>
     <row r="92">
@@ -11695,7 +11695,7 @@
         <v>0</v>
       </c>
       <c r="AJ92" t="n">
-        <v>1.133785606133643</v>
+        <v>0.9724887508473049</v>
       </c>
     </row>
     <row r="93">
@@ -11817,7 +11817,7 @@
         <v>0</v>
       </c>
       <c r="AJ93" t="n">
-        <v>0.5489691652738172</v>
+        <v>0.01570877757925192</v>
       </c>
     </row>
     <row r="94">
@@ -11939,7 +11939,7 @@
         <v>0</v>
       </c>
       <c r="AJ94" t="n">
-        <v>0.5714477987498265</v>
+        <v>0.01632873282142362</v>
       </c>
     </row>
     <row r="95">
@@ -12061,7 +12061,7 @@
         <v>0</v>
       </c>
       <c r="AJ95" t="n">
-        <v>1.151331207154473</v>
+        <v>0.03289591306155636</v>
       </c>
     </row>
     <row r="96">
@@ -12183,7 +12183,7 @@
         <v>0</v>
       </c>
       <c r="AJ96" t="n">
-        <v>0.5176072876491536</v>
+        <v>0.01479187821854725</v>
       </c>
     </row>
     <row r="97">
@@ -12305,7 +12305,7 @@
         <v>0</v>
       </c>
       <c r="AJ97" t="n">
-        <v>0.5114281621647001</v>
+        <v>0.01461710749042</v>
       </c>
     </row>
     <row r="98">
@@ -12427,7 +12427,7 @@
         <v>0</v>
       </c>
       <c r="AJ98" t="n">
-        <v>0.5689422367951569</v>
+        <v>0.01625975962271877</v>
       </c>
     </row>
     <row r="99">
@@ -12549,7 +12549,7 @@
         <v>0</v>
       </c>
       <c r="AJ99" t="n">
-        <v>0.854846036501994</v>
+        <v>0.9690116810215662</v>
       </c>
     </row>
     <row r="100">
@@ -12671,7 +12671,7 @@
         <v>0</v>
       </c>
       <c r="AJ100" t="n">
-        <v>0.6211791757704777</v>
+        <v>0.01775044787915651</v>
       </c>
     </row>
     <row r="101">
@@ -12793,7 +12793,7 @@
         <v>0</v>
       </c>
       <c r="AJ101" t="n">
-        <v>0.7169446472424653</v>
+        <v>0.02048582563549901</v>
       </c>
     </row>
     <row r="102">
@@ -12915,7 +12915,7 @@
         <v>0</v>
       </c>
       <c r="AJ102" t="n">
-        <v>0.9142412960039988</v>
+        <v>0.9677627437257447</v>
       </c>
     </row>
     <row r="103">
@@ -13037,7 +13037,7 @@
         <v>0</v>
       </c>
       <c r="AJ103" t="n">
-        <v>0.452281416162101</v>
+        <v>0.01292392046177432</v>
       </c>
     </row>
     <row r="104">
@@ -13159,7 +13159,7 @@
         <v>0</v>
       </c>
       <c r="AJ104" t="n">
-        <v>0.5210362757839306</v>
+        <v>0.01491069502239802</v>
       </c>
     </row>
     <row r="105">
@@ -13281,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="AJ105" t="n">
-        <v>0.80886799895221</v>
+        <v>0.7209654643830904</v>
       </c>
     </row>
     <row r="106">
@@ -13403,7 +13403,7 @@
         <v>0</v>
       </c>
       <c r="AJ106" t="n">
-        <v>1.129912861801258</v>
+        <v>0.7711708842506289</v>
       </c>
     </row>
     <row r="107">
@@ -13525,7 +13525,7 @@
         <v>0</v>
       </c>
       <c r="AJ107" t="n">
-        <v>0.5644841196571023</v>
+        <v>0.01613127627591721</v>
       </c>
     </row>
     <row r="108">
@@ -13647,7 +13647,7 @@
         <v>0</v>
       </c>
       <c r="AJ108" t="n">
-        <v>0.4656937871216572</v>
+        <v>0.01332948106061878</v>
       </c>
     </row>
     <row r="109">
@@ -13765,7 +13765,7 @@
         <v>0</v>
       </c>
       <c r="AJ109" t="n">
-        <v>0.600361543491741</v>
+        <v>0.01715745409976403</v>
       </c>
     </row>
     <row r="110">
@@ -13887,7 +13887,7 @@
         <v>0</v>
       </c>
       <c r="AJ110" t="n">
-        <v>1.004056651555323</v>
+        <v>0.8609329341973826</v>
       </c>
     </row>
     <row r="111">
@@ -14009,7 +14009,7 @@
         <v>0</v>
       </c>
       <c r="AJ111" t="n">
-        <v>0.719573825711362</v>
+        <v>0.02056412644889605</v>
       </c>
     </row>
     <row r="112">
@@ -14131,7 +14131,7 @@
         <v>0</v>
       </c>
       <c r="AJ112" t="n">
-        <v>1.118709085976296</v>
+        <v>1.337116283268068</v>
       </c>
     </row>
     <row r="113">
@@ -14253,7 +14253,7 @@
         <v>0</v>
       </c>
       <c r="AJ113" t="n">
-        <v>0.5778783922594405</v>
+        <v>0.01651556835026973</v>
       </c>
     </row>
     <row r="114">
@@ -14375,7 +14375,7 @@
         <v>0</v>
       </c>
       <c r="AJ114" t="n">
-        <v>0.9726674402121934</v>
+        <v>1.292619337224446</v>
       </c>
     </row>
     <row r="115">
@@ -14498,7 +14498,7 @@
         <v>0</v>
       </c>
       <c r="AJ115" t="n">
-        <v>0.9923111703348928</v>
+        <v>1.413461968338274</v>
       </c>
     </row>
     <row r="116">
@@ -14620,7 +14620,7 @@
         <v>0</v>
       </c>
       <c r="AJ116" t="n">
-        <v>0.5210362757839306</v>
+        <v>0.01491069502239802</v>
       </c>
     </row>
     <row r="117">
@@ -14742,7 +14742,7 @@
         <v>0</v>
       </c>
       <c r="AJ117" t="n">
-        <v>1.065208408683048</v>
+        <v>1.399612910634444</v>
       </c>
     </row>
     <row r="118">
@@ -14864,7 +14864,7 @@
         <v>0</v>
       </c>
       <c r="AJ118" t="n">
-        <v>0.4072769983905605</v>
+        <v>0.01163817852544459</v>
       </c>
     </row>
     <row r="119">
@@ -14986,7 +14986,7 @@
         <v>0</v>
       </c>
       <c r="AJ119" t="n">
-        <v>0.8723530651995517</v>
+        <v>0.9665689517827384</v>
       </c>
     </row>
     <row r="120">
@@ -15108,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="AJ120" t="n">
-        <v>0.9024456259694505</v>
+        <v>1.096771813328957</v>
       </c>
     </row>
     <row r="121">
@@ -15230,7 +15230,7 @@
         <v>0</v>
       </c>
       <c r="AJ121" t="n">
-        <v>0.457982052776905</v>
+        <v>0.01310914579362586</v>
       </c>
     </row>
     <row r="122">
@@ -15352,7 +15352,7 @@
         <v>0</v>
       </c>
       <c r="AJ122" t="n">
-        <v>0.5909541078555171</v>
+        <v>0.01690834736730049</v>
       </c>
     </row>
     <row r="123">
@@ -15474,7 +15474,7 @@
         <v>0</v>
       </c>
       <c r="AJ123" t="n">
-        <v>1.020556420737196</v>
+        <v>1.260148466433673</v>
       </c>
     </row>
     <row r="124">
@@ -15596,7 +15596,7 @@
         <v>0</v>
       </c>
       <c r="AJ124" t="n">
-        <v>0.5012949743916552</v>
+        <v>0.01432402641119015</v>
       </c>
     </row>
     <row r="125">
@@ -15719,7 +15719,7 @@
         <v>0</v>
       </c>
       <c r="AJ125" t="n">
-        <v>0.5667706508269735</v>
+        <v>0.01619832145219924</v>
       </c>
     </row>
     <row r="126">
@@ -15842,7 +15842,7 @@
         <v>0</v>
       </c>
       <c r="AJ126" t="n">
-        <v>1.099844942089622</v>
+        <v>1.59511082255433</v>
       </c>
     </row>
     <row r="127">
@@ -15964,7 +15964,7 @@
         <v>0</v>
       </c>
       <c r="AJ127" t="n">
-        <v>0.8292806328643229</v>
+        <v>0.9867635820235675</v>
       </c>
     </row>
     <row r="128">
@@ -16086,7 +16086,7 @@
         <v>0</v>
       </c>
       <c r="AJ128" t="n">
-        <v>0.7343624116852916</v>
+        <v>0.0209824117624369</v>
       </c>
     </row>
     <row r="129">
@@ -16208,7 +16208,7 @@
         <v>0</v>
       </c>
       <c r="AJ129" t="n">
-        <v>0.5650906822200967</v>
+        <v>0.01614827663485991</v>
       </c>
     </row>
     <row r="130">
@@ -16330,7 +16330,7 @@
         <v>0</v>
       </c>
       <c r="AJ130" t="n">
-        <v>0.5011381967271197</v>
+        <v>0.01431988704934628</v>
       </c>
     </row>
     <row r="131">
@@ -16452,7 +16452,7 @@
         <v>0</v>
       </c>
       <c r="AJ131" t="n">
-        <v>1.016687616547627</v>
+        <v>0.9738536107606501</v>
       </c>
     </row>
     <row r="132">
@@ -16574,7 +16574,7 @@
         <v>0</v>
       </c>
       <c r="AJ132" t="n">
-        <v>0.5133245414391784</v>
+        <v>0.0146903597554051</v>
       </c>
     </row>
     <row r="133">
@@ -16696,7 +16696,7 @@
         <v>0</v>
       </c>
       <c r="AJ133" t="n">
-        <v>1.032535690400309</v>
+        <v>1.525643076440557</v>
       </c>
     </row>
     <row r="134">
@@ -16818,7 +16818,7 @@
         <v>0</v>
       </c>
       <c r="AJ134" t="n">
-        <v>1.312281891197334</v>
+        <v>1.149694604824694</v>
       </c>
     </row>
     <row r="135">
@@ -16940,7 +16940,7 @@
         <v>0</v>
       </c>
       <c r="AJ135" t="n">
-        <v>1.304241346694348</v>
+        <v>1.080649976589884</v>
       </c>
     </row>
     <row r="136">
@@ -17062,7 +17062,7 @@
         <v>0</v>
       </c>
       <c r="AJ136" t="n">
-        <v>0.7192174240740079</v>
+        <v>0.6779775079261311</v>
       </c>
     </row>
     <row r="137">
@@ -17184,7 +17184,7 @@
         <v>0</v>
       </c>
       <c r="AJ137" t="n">
-        <v>1.292094886049719</v>
+        <v>1.218160616197793</v>
       </c>
     </row>
     <row r="138">
@@ -17306,7 +17306,7 @@
         <v>0</v>
       </c>
       <c r="AJ138" t="n">
-        <v>0.65672585354028</v>
+        <v>0.4086825805272796</v>
       </c>
     </row>
     <row r="139">
@@ -17428,7 +17428,7 @@
         <v>0</v>
       </c>
       <c r="AJ139" t="n">
-        <v>1.180401383396333</v>
+        <v>1.208237642260226</v>
       </c>
     </row>
     <row r="140">
@@ -17550,7 +17550,7 @@
         <v>0</v>
       </c>
       <c r="AJ140" t="n">
-        <v>1.011018668421963</v>
+        <v>1.184869132703341</v>
       </c>
     </row>
     <row r="141">
@@ -17672,7 +17672,7 @@
         <v>0</v>
       </c>
       <c r="AJ141" t="n">
-        <v>0.5599479751927343</v>
+        <v>0.01600278071979241</v>
       </c>
     </row>
     <row r="142">
@@ -17794,7 +17794,7 @@
         <v>0</v>
       </c>
       <c r="AJ142" t="n">
-        <v>0.4750979850556415</v>
+        <v>0.01357874957301833</v>
       </c>
     </row>
     <row r="143">
@@ -17916,7 +17916,7 @@
         <v>0</v>
       </c>
       <c r="AJ143" t="n">
-        <v>0.8959180832627224</v>
+        <v>0.8628298542574676</v>
       </c>
     </row>
     <row r="144">
@@ -18038,7 +18038,7 @@
         <v>0</v>
       </c>
       <c r="AJ144" t="n">
-        <v>1.022290691461426</v>
+        <v>1.156972190350963</v>
       </c>
     </row>
     <row r="145">
@@ -18160,7 +18160,7 @@
         <v>0</v>
       </c>
       <c r="AJ145" t="n">
-        <v>1.298894681509867</v>
+        <v>1.28481640581524</v>
       </c>
     </row>
     <row r="146">
@@ -18282,7 +18282,7 @@
         <v>0</v>
       </c>
       <c r="AJ146" t="n">
-        <v>0.6391514885395416</v>
+        <v>0.01826316395827262</v>
       </c>
     </row>
     <row r="147">
@@ -18404,7 +18404,7 @@
         <v>0</v>
       </c>
       <c r="AJ147" t="n">
-        <v>0.5584571631136026</v>
+        <v>0.01596018608896008</v>
       </c>
     </row>
     <row r="148">
@@ -18526,7 +18526,7 @@
         <v>0</v>
       </c>
       <c r="AJ148" t="n">
-        <v>0.9927056525554573</v>
+        <v>1.236120914472183</v>
       </c>
     </row>
     <row r="149">
@@ -18648,7 +18648,7 @@
         <v>0</v>
       </c>
       <c r="AJ149" t="n">
-        <v>0.5387493620989362</v>
+        <v>0.01539566748854104</v>
       </c>
     </row>
     <row r="150">
@@ -18770,7 +18770,7 @@
         <v>0</v>
       </c>
       <c r="AJ150" t="n">
-        <v>0.9597242146484091</v>
+        <v>1.296523526517297</v>
       </c>
     </row>
     <row r="151">
@@ -18892,7 +18892,7 @@
         <v>0</v>
       </c>
       <c r="AJ151" t="n">
-        <v>0.5713842053160997</v>
+        <v>0.01632784586617428</v>
       </c>
     </row>
     <row r="152">
@@ -19014,7 +19014,7 @@
         <v>0</v>
       </c>
       <c r="AJ152" t="n">
-        <v>0.5714385053160996</v>
+        <v>0.01632965586617428</v>
       </c>
     </row>
     <row r="153">
@@ -19136,7 +19136,7 @@
         <v>0</v>
       </c>
       <c r="AJ153" t="n">
-        <v>1.232697303836056</v>
+        <v>1.521794830396569</v>
       </c>
     </row>
     <row r="154">
@@ -19258,7 +19258,7 @@
         <v>0</v>
       </c>
       <c r="AJ154" t="n">
-        <v>1.008649783030582</v>
+        <v>1.074661496724647</v>
       </c>
     </row>
     <row r="155">
@@ -19380,7 +19380,7 @@
         <v>0</v>
       </c>
       <c r="AJ155" t="n">
-        <v>0.7299391010364541</v>
+        <v>0.02085614574389869</v>
       </c>
     </row>
     <row r="156">
@@ -19502,7 +19502,7 @@
         <v>0</v>
       </c>
       <c r="AJ156" t="n">
-        <v>1.182154006773891</v>
+        <v>0.8604913757402232</v>
       </c>
     </row>
     <row r="157">
@@ -19624,7 +19624,7 @@
         <v>0</v>
       </c>
       <c r="AJ157" t="n">
-        <v>0.8955210914472896</v>
+        <v>1.000875275048335</v>
       </c>
     </row>
     <row r="158">
@@ -19746,7 +19746,7 @@
         <v>0</v>
       </c>
       <c r="AJ158" t="n">
-        <v>0.4929430812763994</v>
+        <v>0.01408574089361141</v>
       </c>
     </row>
     <row r="159">
@@ -19868,7 +19868,7 @@
         <v>0</v>
       </c>
       <c r="AJ159" t="n">
-        <v>0.6955193397648095</v>
+        <v>0.01987533827899456</v>
       </c>
     </row>
     <row r="160">
@@ -19990,7 +19990,7 @@
         <v>0</v>
       </c>
       <c r="AJ160" t="n">
-        <v>0.480009083342415</v>
+        <v>0.01371881238121186</v>
       </c>
     </row>
     <row r="161">
@@ -20112,7 +20112,7 @@
         <v>0</v>
       </c>
       <c r="AJ161" t="n">
-        <v>1.21721507069691</v>
+        <v>0.03478043344848313</v>
       </c>
     </row>
     <row r="162">
@@ -20234,7 +20234,7 @@
         <v>0</v>
       </c>
       <c r="AJ162" t="n">
-        <v>0.968378915642224</v>
+        <v>1.093071893436562</v>
       </c>
     </row>
     <row r="163">
@@ -20356,7 +20356,7 @@
         <v>0</v>
       </c>
       <c r="AJ163" t="n">
-        <v>1.259174966413742</v>
+        <v>1.248053234020284</v>
       </c>
     </row>
     <row r="164">
@@ -20478,7 +20478,7 @@
         <v>0</v>
       </c>
       <c r="AJ164" t="n">
-        <v>1.030748053161446</v>
+        <v>1.321423155270638</v>
       </c>
     </row>
     <row r="165">
@@ -20600,7 +20600,7 @@
         <v>0</v>
       </c>
       <c r="AJ165" t="n">
-        <v>1.076561569979037</v>
+        <v>0.9691409079813067</v>
       </c>
     </row>
     <row r="166">
@@ -20722,7 +20722,7 @@
         <v>0</v>
       </c>
       <c r="AJ166" t="n">
-        <v>1.24317055395123</v>
+        <v>0.9816578738183556</v>
       </c>
     </row>
     <row r="167">
@@ -20840,7 +20840,7 @@
         <v>0</v>
       </c>
       <c r="AJ167" t="n">
-        <v>1.964031655474045</v>
+        <v>1.615626467328572</v>
       </c>
     </row>
     <row r="168">
@@ -20962,7 +20962,7 @@
         <v>0</v>
       </c>
       <c r="AJ168" t="n">
-        <v>1.038235879314084</v>
+        <v>1.407784774931897</v>
       </c>
     </row>
     <row r="169">
@@ -21084,7 +21084,7 @@
         <v>0</v>
       </c>
       <c r="AJ169" t="n">
-        <v>1.062314801659158</v>
+        <v>1.374775091351096</v>
       </c>
     </row>
     <row r="170">
@@ -21206,7 +21206,7 @@
         <v>0</v>
       </c>
       <c r="AJ170" t="n">
-        <v>1.261940642036995</v>
+        <v>1.248386134151293</v>
       </c>
     </row>
     <row r="171">
@@ -21324,7 +21324,7 @@
         <v>0</v>
       </c>
       <c r="AJ171" t="n">
-        <v>0.8672474105628644</v>
+        <v>0.9590947839805734</v>
       </c>
     </row>
     <row r="172">
@@ -21446,7 +21446,7 @@
         <v>0</v>
       </c>
       <c r="AJ172" t="n">
-        <v>0.8921349857185163</v>
+        <v>0.8524023511336905</v>
       </c>
     </row>
     <row r="173">
@@ -21568,7 +21568,7 @@
         <v>0</v>
       </c>
       <c r="AJ173" t="n">
-        <v>1.116409022090248</v>
+        <v>1.613267756209385</v>
       </c>
     </row>
     <row r="174">
@@ -21690,7 +21690,7 @@
         <v>0</v>
       </c>
       <c r="AJ174" t="n">
-        <v>1.087295464193757</v>
+        <v>1.532109252766558</v>
       </c>
     </row>
     <row r="175">
@@ -21808,7 +21808,7 @@
         <v>0</v>
       </c>
       <c r="AJ175" t="n">
-        <v>1.092287690887407</v>
+        <v>1.426201954734972</v>
       </c>
     </row>
     <row r="176">
@@ -21930,7 +21930,7 @@
         <v>0</v>
       </c>
       <c r="AJ176" t="n">
-        <v>0.4807584997875926</v>
+        <v>0.01373627142250265</v>
       </c>
     </row>
     <row r="177">
@@ -22052,7 +22052,7 @@
         <v>0</v>
       </c>
       <c r="AJ177" t="n">
-        <v>1.028678649568016</v>
+        <v>1.410298813194996</v>
       </c>
     </row>
     <row r="178">
@@ -22174,7 +22174,7 @@
         <v>0</v>
       </c>
       <c r="AJ178" t="n">
-        <v>0.8611104947337772</v>
+        <v>0.02460533127810792</v>
       </c>
     </row>
     <row r="179">
@@ -22296,7 +22296,7 @@
         <v>0</v>
       </c>
       <c r="AJ179" t="n">
-        <v>1.042644113511559</v>
+        <v>1.091056016855246</v>
       </c>
     </row>
     <row r="180">
@@ -22418,7 +22418,7 @@
         <v>0</v>
       </c>
       <c r="AJ180" t="n">
-        <v>1.114794697415507</v>
+        <v>1.117084938608608</v>
       </c>
     </row>
     <row r="181">
@@ -22540,7 +22540,7 @@
         <v>0</v>
       </c>
       <c r="AJ181" t="n">
-        <v>1.264143300937408</v>
+        <v>1.615208797346987</v>
       </c>
     </row>
     <row r="182">
@@ -22662,7 +22662,7 @@
         <v>0</v>
       </c>
       <c r="AJ182" t="n">
-        <v>0.9180126324793884</v>
+        <v>0.9835467494506185</v>
       </c>
     </row>
     <row r="183">
@@ -22784,7 +22784,7 @@
         <v>0</v>
       </c>
       <c r="AJ183" t="n">
-        <v>0.5493493270829753</v>
+        <v>0.01570744934522787</v>
       </c>
     </row>
     <row r="184">
@@ -22906,7 +22906,7 @@
         <v>0</v>
       </c>
       <c r="AJ184" t="n">
-        <v>0.8781943521778173</v>
+        <v>0.9698263622259781</v>
       </c>
     </row>
     <row r="185">
@@ -23028,7 +23028,7 @@
         <v>0</v>
       </c>
       <c r="AJ185" t="n">
-        <v>0.6855703529077903</v>
+        <v>0.01958858579736544</v>
       </c>
     </row>
     <row r="186">
@@ -23150,7 +23150,7 @@
         <v>0</v>
       </c>
       <c r="AJ186" t="n">
-        <v>1.283394355303417</v>
+        <v>1.602390073811615</v>
       </c>
     </row>
     <row r="187">
@@ -23272,7 +23272,7 @@
         <v>0</v>
       </c>
       <c r="AJ187" t="n">
-        <v>0.9516693443073232</v>
+        <v>0.9977734533047647</v>
       </c>
     </row>
     <row r="188">
@@ -23394,7 +23394,7 @@
         <v>0</v>
       </c>
       <c r="AJ188" t="n">
-        <v>0.5693804423685486</v>
+        <v>0.01627976692481567</v>
       </c>
     </row>
     <row r="189">
@@ -23516,7 +23516,7 @@
         <v>0</v>
       </c>
       <c r="AJ189" t="n">
-        <v>1.037143462269946</v>
+        <v>0.9679485927566345</v>
       </c>
     </row>
     <row r="190">
@@ -23638,7 +23638,7 @@
         <v>0</v>
       </c>
       <c r="AJ190" t="n">
-        <v>0.6620406292678768</v>
+        <v>0.01892474226479648</v>
       </c>
     </row>
     <row r="191">
@@ -23760,7 +23760,7 @@
         <v>0</v>
       </c>
       <c r="AJ191" t="n">
-        <v>0.9845834376587046</v>
+        <v>1.156247472012267</v>
       </c>
     </row>
     <row r="192">
@@ -23878,7 +23878,7 @@
         <v>0</v>
       </c>
       <c r="AJ192" t="n">
-        <v>0.962124720927151</v>
+        <v>1.184007045923158</v>
       </c>
     </row>
     <row r="193">
@@ -24000,7 +24000,7 @@
         <v>0</v>
       </c>
       <c r="AJ193" t="n">
-        <v>1.603139258297761</v>
+        <v>1.113108271111955</v>
       </c>
     </row>
     <row r="194">
@@ -24122,7 +24122,7 @@
         <v>0</v>
       </c>
       <c r="AJ194" t="n">
-        <v>0.994993339245444</v>
+        <v>0.9746153650026612</v>
       </c>
     </row>
     <row r="195">
@@ -24244,7 +24244,7 @@
         <v>0</v>
       </c>
       <c r="AJ195" t="n">
-        <v>1.219961243335304</v>
+        <v>0.9795642540262646</v>
       </c>
     </row>
     <row r="196">
@@ -24366,7 +24366,7 @@
         <v>0</v>
       </c>
       <c r="AJ196" t="n">
-        <v>1.151849702980694</v>
+        <v>0.7307639202124757</v>
       </c>
     </row>
     <row r="197">
@@ -24488,7 +24488,7 @@
         <v>0</v>
       </c>
       <c r="AJ197" t="n">
-        <v>0.7959827745004382</v>
+        <v>0.7409461261150154</v>
       </c>
     </row>
     <row r="198">
@@ -24610,7 +24610,7 @@
         <v>0</v>
       </c>
       <c r="AJ198" t="n">
-        <v>0.9092042553966562</v>
+        <v>0.4207612118862868</v>
       </c>
     </row>
     <row r="199">
@@ -24732,7 +24732,7 @@
         <v>0</v>
       </c>
       <c r="AJ199" t="n">
-        <v>1.179243524875816</v>
+        <v>1.205292603522163</v>
       </c>
     </row>
     <row r="200">
@@ -24854,7 +24854,7 @@
         <v>0</v>
       </c>
       <c r="AJ200" t="n">
-        <v>0.6073260270965198</v>
+        <v>0.017365226488472</v>
       </c>
     </row>
     <row r="201">
@@ -24976,7 +24976,7 @@
         <v>0</v>
       </c>
       <c r="AJ201" t="n">
-        <v>1.04076385723445</v>
+        <v>1.065632786507517</v>
       </c>
     </row>
     <row r="202">
@@ -25098,7 +25098,7 @@
         <v>0</v>
       </c>
       <c r="AJ202" t="n">
-        <v>0.7500670799655079</v>
+        <v>0.3987202225651327</v>
       </c>
     </row>
     <row r="203">
@@ -25220,7 +25220,7 @@
         <v>0</v>
       </c>
       <c r="AJ203" t="n">
-        <v>0.6124765298088261</v>
+        <v>0.01750289656596646</v>
       </c>
     </row>
     <row r="204">
@@ -25342,7 +25342,7 @@
         <v>0</v>
       </c>
       <c r="AJ204" t="n">
-        <v>1.311939934839388</v>
+        <v>1.511052150696285</v>
       </c>
     </row>
     <row r="205">
@@ -25464,7 +25464,7 @@
         <v>0</v>
       </c>
       <c r="AJ205" t="n">
-        <v>0.9914017713695138</v>
+        <v>1.265878256739132</v>
       </c>
     </row>
     <row r="206">
@@ -25586,7 +25586,7 @@
         <v>0</v>
       </c>
       <c r="AJ206" t="n">
-        <v>0.7767419092088824</v>
+        <v>0.8542827692994518</v>
       </c>
     </row>
     <row r="207">
@@ -25708,7 +25708,7 @@
         <v>0</v>
       </c>
       <c r="AJ207" t="n">
-        <v>1.177566775237284</v>
+        <v>1.532239734526648</v>
       </c>
     </row>
     <row r="208">
@@ -25830,7 +25830,7 @@
         <v>0</v>
       </c>
       <c r="AJ208" t="n">
-        <v>0.8274137366686145</v>
+        <v>0.9619263112208366</v>
       </c>
     </row>
     <row r="209">
@@ -25952,7 +25952,7 @@
         <v>0</v>
       </c>
       <c r="AJ209" t="n">
-        <v>0.941324172998566</v>
+        <v>1.206539010303693</v>
       </c>
     </row>
     <row r="210">
@@ -26074,7 +26074,7 @@
         <v>0</v>
       </c>
       <c r="AJ210" t="n">
-        <v>1.308913371664553</v>
+        <v>1.634645270291242</v>
       </c>
     </row>
     <row r="211">
@@ -26196,7 +26196,7 @@
         <v>0</v>
       </c>
       <c r="AJ211" t="n">
-        <v>1.093586358015153</v>
+        <v>1.600986385000881</v>
       </c>
     </row>
     <row r="212">
@@ -26318,7 +26318,7 @@
         <v>0</v>
       </c>
       <c r="AJ212" t="n">
-        <v>0.7048679547272184</v>
+        <v>0.02014024299220624</v>
       </c>
     </row>
     <row r="213">
@@ -26440,7 +26440,7 @@
         <v>0</v>
       </c>
       <c r="AJ213" t="n">
-        <v>1.043246314175693</v>
+        <v>0.971604057853856</v>
       </c>
     </row>
     <row r="214">
@@ -26562,7 +26562,7 @@
         <v>0</v>
       </c>
       <c r="AJ214" t="n">
-        <v>0.5752083147498241</v>
+        <v>0.01644627756428069</v>
       </c>
     </row>
     <row r="215">
@@ -26684,7 +26684,7 @@
         <v>0</v>
       </c>
       <c r="AJ215" t="n">
-        <v>0.7664756922205411</v>
+        <v>1.090253789470074</v>
       </c>
     </row>
     <row r="216">
@@ -26806,7 +26806,7 @@
         <v>0</v>
       </c>
       <c r="AJ216" t="n">
-        <v>0.8427993487826571</v>
+        <v>0.02408210425093306</v>
       </c>
     </row>
     <row r="217">
@@ -26928,7 +26928,7 @@
         <v>0</v>
       </c>
       <c r="AJ217" t="n">
-        <v>1.401781574360845</v>
+        <v>0.9818921065560074</v>
       </c>
     </row>
     <row r="218">
@@ -27050,7 +27050,7 @@
         <v>0</v>
       </c>
       <c r="AJ218" t="n">
-        <v>0.8947324135308016</v>
+        <v>0.8678888070567096</v>
       </c>
     </row>
     <row r="219">
@@ -27172,7 +27172,7 @@
         <v>0</v>
       </c>
       <c r="AJ219" t="n">
-        <v>0.8040888728153683</v>
+        <v>0.9593901090813427</v>
       </c>
     </row>
     <row r="220">
@@ -27294,7 +27294,7 @@
         <v>0</v>
       </c>
       <c r="AJ220" t="n">
-        <v>1.072011744695874</v>
+        <v>0.7002179768966335</v>
       </c>
     </row>
     <row r="221">
@@ -27416,7 +27416,7 @@
         <v>0</v>
       </c>
       <c r="AJ221" t="n">
-        <v>0.8585762082861601</v>
+        <v>0.02453129452246172</v>
       </c>
     </row>
     <row r="222">
@@ -27538,7 +27538,7 @@
         <v>0</v>
       </c>
       <c r="AJ222" t="n">
-        <v>0.8107516240320719</v>
+        <v>0.4155202849089263</v>
       </c>
     </row>
     <row r="223">
@@ -27660,7 +27660,7 @@
         <v>0</v>
       </c>
       <c r="AJ223" t="n">
-        <v>0.9049752658979798</v>
+        <v>1.049567029217732</v>
       </c>
     </row>
     <row r="224">
@@ -27782,7 +27782,7 @@
         <v>0</v>
       </c>
       <c r="AJ224" t="n">
-        <v>0.9517456958048289</v>
+        <v>1.249480771682781</v>
       </c>
     </row>
     <row r="225">
@@ -27904,7 +27904,7 @@
         <v>0</v>
       </c>
       <c r="AJ225" t="n">
-        <v>1.225069473655116</v>
+        <v>1.078745428380814</v>
       </c>
     </row>
     <row r="226">
@@ -28026,7 +28026,7 @@
         <v>0</v>
       </c>
       <c r="AJ226" t="n">
-        <v>1.28991781430695</v>
+        <v>1.098118164020829</v>
       </c>
     </row>
     <row r="227">
@@ -28144,7 +28144,7 @@
         <v>0</v>
       </c>
       <c r="AJ227" t="n">
-        <v>1.453744239061178</v>
+        <v>1.33376272695279</v>
       </c>
     </row>
     <row r="228">
@@ -28266,7 +28266,7 @@
         <v>0</v>
       </c>
       <c r="AJ228" t="n">
-        <v>1.270020136638994</v>
+        <v>0.03628767390397126</v>
       </c>
     </row>
     <row r="229">
@@ -28388,7 +28388,7 @@
         <v>0</v>
       </c>
       <c r="AJ229" t="n">
-        <v>1.158599945218142</v>
+        <v>1.415004578154642</v>
       </c>
     </row>
     <row r="230">
@@ -28506,7 +28506,7 @@
         <v>0</v>
       </c>
       <c r="AJ230" t="n">
-        <v>1.021088207590029</v>
+        <v>1.154499347620929</v>
       </c>
     </row>
     <row r="231">
@@ -28628,7 +28628,7 @@
         <v>0</v>
       </c>
       <c r="AJ231" t="n">
-        <v>1.22460440855272</v>
+        <v>1.535943116236262</v>
       </c>
     </row>
     <row r="232">
@@ -28750,7 +28750,7 @@
         <v>0</v>
       </c>
       <c r="AJ232" t="n">
-        <v>1.485127204333648</v>
+        <v>1.438913285699949</v>
       </c>
     </row>
     <row r="233">
@@ -28868,7 +28868,7 @@
         <v>0</v>
       </c>
       <c r="AJ233" t="n">
-        <v>0.8677485536578149</v>
+        <v>0.8669250514779129</v>
       </c>
     </row>
     <row r="234">
@@ -28990,7 +28990,7 @@
         <v>0</v>
       </c>
       <c r="AJ234" t="n">
-        <v>0.938488747690586</v>
+        <v>0.8474198456845358</v>
       </c>
     </row>
     <row r="235">
@@ -29112,7 +29112,7 @@
         <v>0</v>
       </c>
       <c r="AJ235" t="n">
-        <v>1.137021205962226</v>
+        <v>1.073235411343881</v>
       </c>
     </row>
     <row r="236">
@@ -29234,7 +29234,7 @@
         <v>0</v>
       </c>
       <c r="AJ236" t="n">
-        <v>0.8198439842032866</v>
+        <v>0.8606559342843408</v>
       </c>
     </row>
     <row r="237">
@@ -29356,7 +29356,7 @@
         <v>0</v>
       </c>
       <c r="AJ237" t="n">
-        <v>0.9852854116914377</v>
+        <v>0.9664238173810559</v>
       </c>
     </row>
     <row r="238">
@@ -29478,7 +29478,7 @@
         <v>0</v>
       </c>
       <c r="AJ238" t="n">
-        <v>1.118216284731881</v>
+        <v>0.03195042099233945</v>
       </c>
     </row>
     <row r="239">
@@ -29600,7 +29600,7 @@
         <v>0</v>
       </c>
       <c r="AJ239" t="n">
-        <v>0.9966120914960725</v>
+        <v>0.9858915064832439</v>
       </c>
     </row>
     <row r="240">
@@ -29722,7 +29722,7 @@
         <v>0</v>
       </c>
       <c r="AJ240" t="n">
-        <v>0.6870701404433274</v>
+        <v>0.01964362972695221</v>
       </c>
     </row>
     <row r="241">
@@ -29844,7 +29844,7 @@
         <v>0</v>
       </c>
       <c r="AJ241" t="n">
-        <v>0.8982997702422297</v>
+        <v>0.02567876200692085</v>
       </c>
     </row>
     <row r="242">
@@ -29966,7 +29966,7 @@
         <v>0</v>
       </c>
       <c r="AJ242" t="n">
-        <v>0.8218744425936478</v>
+        <v>0.8657428810599102</v>
       </c>
     </row>
     <row r="243">
@@ -30084,7 +30084,7 @@
         <v>0</v>
       </c>
       <c r="AJ243" t="n">
-        <v>1.210828649473102</v>
+        <v>1.591219061842543</v>
       </c>
     </row>
     <row r="244">
@@ -30202,7 +30202,7 @@
         <v>0</v>
       </c>
       <c r="AJ244" t="n">
-        <v>0.574376573666188</v>
+        <v>0.01642251353331966</v>
       </c>
     </row>
     <row r="245">
@@ -30324,7 +30324,7 @@
         <v>0</v>
       </c>
       <c r="AJ245" t="n">
-        <v>0.8626243199983854</v>
+        <v>0.9665510926220671</v>
       </c>
     </row>
     <row r="246">
@@ -30446,7 +30446,7 @@
         <v>0</v>
       </c>
       <c r="AJ246" t="n">
-        <v>0.8244295038502996</v>
+        <v>0.9939670921980609</v>
       </c>
     </row>
     <row r="247">
@@ -30568,7 +30568,7 @@
         <v>0</v>
       </c>
       <c r="AJ247" t="n">
-        <v>0.5119005939425478</v>
+        <v>0.01462711554121565</v>
       </c>
     </row>
     <row r="248">
@@ -30686,7 +30686,7 @@
         <v>0</v>
       </c>
       <c r="AJ248" t="n">
-        <v>1.670814005289333</v>
+        <v>1.424369661032377</v>
       </c>
     </row>
     <row r="249">
@@ -30808,7 +30808,7 @@
         <v>0</v>
       </c>
       <c r="AJ249" t="n">
-        <v>1.007226487785097</v>
+        <v>1.275886049454925</v>
       </c>
     </row>
     <row r="250">
@@ -30926,7 +30926,7 @@
         <v>0</v>
       </c>
       <c r="AJ250" t="n">
-        <v>0.5952724281006821</v>
+        <v>0.01702083794573378</v>
       </c>
     </row>
     <row r="251">
@@ -31048,7 +31048,7 @@
         <v>0</v>
       </c>
       <c r="AJ251" t="n">
-        <v>0.7410263409708236</v>
+        <v>0.02117411688488068</v>
       </c>
     </row>
     <row r="252">
@@ -31170,7 +31170,7 @@
         <v>0</v>
       </c>
       <c r="AJ252" t="n">
-        <v>1.05910464322543</v>
+        <v>1.535257701645699</v>
       </c>
     </row>
     <row r="253">
@@ -31288,7 +31288,7 @@
         <v>0</v>
       </c>
       <c r="AJ253" t="n">
-        <v>1.04307810846249</v>
+        <v>0.9945528330549237</v>
       </c>
     </row>
     <row r="254">
@@ -31410,7 +31410,7 @@
         <v>0</v>
       </c>
       <c r="AJ254" t="n">
-        <v>1.752140308894385</v>
+        <v>1.312042649334271</v>
       </c>
     </row>
     <row r="255">
@@ -31528,7 +31528,7 @@
         <v>0</v>
       </c>
       <c r="AJ255" t="n">
-        <v>1.484482930303925</v>
+        <v>1.002614483756595</v>
       </c>
     </row>
     <row r="256">
@@ -31650,7 +31650,7 @@
         <v>0</v>
       </c>
       <c r="AJ256" t="n">
-        <v>1.55753139728274</v>
+        <v>1.313585080883776</v>
       </c>
     </row>
     <row r="257">
@@ -31772,7 +31772,7 @@
         <v>0</v>
       </c>
       <c r="AJ257" t="n">
-        <v>1.152834597631776</v>
+        <v>1.513858762005208</v>
       </c>
     </row>
     <row r="258">
@@ -31894,7 +31894,7 @@
         <v>0</v>
       </c>
       <c r="AJ258" t="n">
-        <v>0.5298543171559615</v>
+        <v>0.0151400790615989</v>
       </c>
     </row>
     <row r="259">
@@ -32016,7 +32016,7 @@
         <v>0</v>
       </c>
       <c r="AJ259" t="n">
-        <v>1.064011905752107</v>
+        <v>0.03040963587863164</v>
       </c>
     </row>
     <row r="260">
@@ -32138,7 +32138,7 @@
         <v>0</v>
       </c>
       <c r="AJ260" t="n">
-        <v>1.404736149359591</v>
+        <v>1.41546053071297</v>
       </c>
     </row>
     <row r="261">
@@ -32260,7 +32260,7 @@
         <v>0</v>
       </c>
       <c r="AJ261" t="n">
-        <v>1.071890522132956</v>
+        <v>0.9768092274397078</v>
       </c>
     </row>
     <row r="262">
@@ -32382,7 +32382,7 @@
         <v>0</v>
       </c>
       <c r="AJ262" t="n">
-        <v>1.070081128249043</v>
+        <v>1.323094297788953</v>
       </c>
     </row>
     <row r="263">
@@ -32500,7 +32500,7 @@
         <v>0</v>
       </c>
       <c r="AJ263" t="n">
-        <v>0.9564990595481661</v>
+        <v>1.120261506549991</v>
       </c>
     </row>
     <row r="264">
@@ -32622,7 +32622,7 @@
         <v>0</v>
       </c>
       <c r="AJ264" t="n">
-        <v>1.273417468262814</v>
+        <v>0.03639672766465183</v>
       </c>
     </row>
     <row r="265">
@@ -32744,7 +32744,7 @@
         <v>0</v>
       </c>
       <c r="AJ265" t="n">
-        <v>1.583885114706084</v>
+        <v>1.258327956540205</v>
       </c>
     </row>
     <row r="266">
@@ -32866,7 +32866,7 @@
         <v>0</v>
       </c>
       <c r="AJ266" t="n">
-        <v>0.6408414623004962</v>
+        <v>0.01832281035144275</v>
       </c>
     </row>
     <row r="267">
@@ -32988,7 +32988,7 @@
         <v>0</v>
       </c>
       <c r="AJ267" t="n">
-        <v>0.7456485200474189</v>
+        <v>0.02131599771564054</v>
       </c>
     </row>
     <row r="268">
@@ -33110,7 +33110,7 @@
         <v>0</v>
       </c>
       <c r="AJ268" t="n">
-        <v>0.4441533877763365</v>
+        <v>0.0127031510793239</v>
       </c>
     </row>
     <row r="269">
@@ -33232,7 +33232,7 @@
         <v>0</v>
       </c>
       <c r="AJ269" t="n">
-        <v>0.6195209406881342</v>
+        <v>0.01770127116251812</v>
       </c>
     </row>
     <row r="270">
@@ -33350,7 +33350,7 @@
         <v>0</v>
       </c>
       <c r="AJ270" t="n">
-        <v>1.018483709652437</v>
+        <v>1.422185577641318</v>
       </c>
     </row>
     <row r="271">
@@ -33468,7 +33468,7 @@
         <v>0</v>
       </c>
       <c r="AJ271" t="n">
-        <v>0.8716246072191411</v>
+        <v>0.9746914255453266</v>
       </c>
     </row>
     <row r="272">
@@ -33586,7 +33586,7 @@
         <v>0</v>
       </c>
       <c r="AJ272" t="n">
-        <v>1.057492714214209</v>
+        <v>1.265394962901039</v>
       </c>
     </row>
     <row r="273">
@@ -33708,7 +33708,7 @@
         <v>0</v>
       </c>
       <c r="AJ273" t="n">
-        <v>0.9006654482491896</v>
+        <v>0.9787884452974089</v>
       </c>
     </row>
     <row r="274">
@@ -33830,7 +33830,7 @@
         <v>0</v>
       </c>
       <c r="AJ274" t="n">
-        <v>0.7029392349438984</v>
+        <v>0.02009734956982567</v>
       </c>
     </row>
     <row r="275">
@@ -33952,7 +33952,7 @@
         <v>0</v>
       </c>
       <c r="AJ275" t="n">
-        <v>1.161964092025354</v>
+        <v>1.634934510119727</v>
       </c>
     </row>
     <row r="276">
@@ -34074,7 +34074,7 @@
         <v>0</v>
       </c>
       <c r="AJ276" t="n">
-        <v>0.9553723901705088</v>
+        <v>1.302475271490294</v>
       </c>
     </row>
     <row r="277">
@@ -34196,7 +34196,7 @@
         <v>0</v>
       </c>
       <c r="AJ277" t="n">
-        <v>1.059679289621107</v>
+        <v>1.15560163567896</v>
       </c>
     </row>
     <row r="278">
@@ -34318,7 +34318,7 @@
         <v>0</v>
       </c>
       <c r="AJ278" t="n">
-        <v>0.6418533148213056</v>
+        <v>0.0183479618520373</v>
       </c>
     </row>
     <row r="279">
@@ -34436,7 +34436,7 @@
         <v>0</v>
       </c>
       <c r="AJ279" t="n">
-        <v>0.9942151031752935</v>
+        <v>1.348330589520624</v>
       </c>
     </row>
     <row r="280">
@@ -34558,7 +34558,7 @@
         <v>0</v>
       </c>
       <c r="AJ280" t="n">
-        <v>1.280857585305937</v>
+        <v>1.156769878429408</v>
       </c>
     </row>
     <row r="281">
@@ -34676,7 +34676,7 @@
         <v>0</v>
       </c>
       <c r="AJ281" t="n">
-        <v>0.8693378582111183</v>
+        <v>0.02483853737746053</v>
       </c>
     </row>
     <row r="282">
@@ -34798,7 +34798,7 @@
         <v>0</v>
       </c>
       <c r="AJ282" t="n">
-        <v>0.8496260872269021</v>
+        <v>0.7423937034057914</v>
       </c>
     </row>
     <row r="283">
@@ -34916,7 +34916,7 @@
         <v>0</v>
       </c>
       <c r="AJ283" t="n">
-        <v>1.334836588534</v>
+        <v>1.330365098366299</v>
       </c>
     </row>
     <row r="284">
@@ -35034,7 +35034,7 @@
         <v>0</v>
       </c>
       <c r="AJ284" t="n">
-        <v>1.276735244073863</v>
+        <v>0.9864071461530131</v>
       </c>
     </row>
     <row r="285">
@@ -35156,7 +35156,7 @@
         <v>0</v>
       </c>
       <c r="AJ285" t="n">
-        <v>1.079006148022382</v>
+        <v>0.03083013137206805</v>
       </c>
     </row>
     <row r="286">
@@ -35274,7 +35274,7 @@
         <v>0</v>
       </c>
       <c r="AJ286" t="n">
-        <v>0.7968519021308089</v>
+        <v>0.757309202431375</v>
       </c>
     </row>
     <row r="287">
@@ -35396,7 +35396,7 @@
         <v>0</v>
       </c>
       <c r="AJ287" t="n">
-        <v>0.8780729159532018</v>
+        <v>0.02510116902723434</v>
       </c>
     </row>
     <row r="288">
@@ -35518,7 +35518,7 @@
         <v>0</v>
       </c>
       <c r="AJ288" t="n">
-        <v>1.033591782807263</v>
+        <v>1.517574399876624</v>
       </c>
     </row>
     <row r="289">
@@ -35640,7 +35640,7 @@
         <v>0</v>
       </c>
       <c r="AJ289" t="n">
-        <v>1.298392716399561</v>
+        <v>1.297538550809967</v>
       </c>
     </row>
     <row r="290">
@@ -35762,7 +35762,7 @@
         <v>0</v>
       </c>
       <c r="AJ290" t="n">
-        <v>1.097517601353492</v>
+        <v>0.03137101718152834</v>
       </c>
     </row>
     <row r="291">
@@ -35884,7 +35884,7 @@
         <v>0</v>
       </c>
       <c r="AJ291" t="n">
-        <v>1.066876368751342</v>
+        <v>1.152167882429627</v>
       </c>
     </row>
     <row r="292">
@@ -36006,7 +36006,7 @@
         <v>0</v>
       </c>
       <c r="AJ292" t="n">
-        <v>0.5185872287327902</v>
+        <v>0.01482058224950829</v>
       </c>
     </row>
     <row r="293">
@@ -36128,7 +36128,7 @@
         <v>0</v>
       </c>
       <c r="AJ293" t="n">
-        <v>0.8872168782323948</v>
+        <v>0.9616892344378931</v>
       </c>
     </row>
     <row r="294">
@@ -36250,7 +36250,7 @@
         <v>0</v>
       </c>
       <c r="AJ294" t="n">
-        <v>1.053457501562895</v>
+        <v>1.412703756449384</v>
       </c>
     </row>
     <row r="295">
@@ -36368,7 +36368,7 @@
         <v>0</v>
       </c>
       <c r="AJ295" t="n">
-        <v>1.258627330048444</v>
+        <v>1.621546003610391</v>
       </c>
     </row>
     <row r="296">
@@ -36490,7 +36490,7 @@
         <v>0</v>
       </c>
       <c r="AJ296" t="n">
-        <v>1.261645824235798</v>
+        <v>0.994219571237961</v>
       </c>
     </row>
     <row r="297">
@@ -36612,7 +36612,7 @@
         <v>0</v>
       </c>
       <c r="AJ297" t="n">
-        <v>1.017773488006684</v>
+        <v>0.02909261394304813</v>
       </c>
     </row>
     <row r="298">
@@ -36734,7 +36734,7 @@
         <v>0</v>
       </c>
       <c r="AJ298" t="n">
-        <v>0.8914445648251489</v>
+        <v>1.25147191121044</v>
       </c>
     </row>
     <row r="299">
@@ -36852,7 +36852,7 @@
         <v>0</v>
       </c>
       <c r="AJ299" t="n">
-        <v>0.7143846321928699</v>
+        <v>0.02041148806265343</v>
       </c>
     </row>
     <row r="300">
@@ -36975,7 +36975,7 @@
         <v>0</v>
       </c>
       <c r="AJ300" t="n">
-        <v>0.5008576967271197</v>
+        <v>0.01431053704934628</v>
       </c>
     </row>
     <row r="301">
@@ -37093,7 +37093,7 @@
         <v>0</v>
       </c>
       <c r="AJ301" t="n">
-        <v>1.01157591346994</v>
+        <v>1.38272921691675</v>
       </c>
     </row>
     <row r="302">
@@ -37211,7 +37211,7 @@
         <v>0</v>
       </c>
       <c r="AJ302" t="n">
-        <v>1.214338162982603</v>
+        <v>1.303558420221165</v>
       </c>
     </row>
     <row r="303">
@@ -37333,7 +37333,7 @@
         <v>0</v>
       </c>
       <c r="AJ303" t="n">
-        <v>1.477294849657589</v>
+        <v>1.282431606739529</v>
       </c>
     </row>
     <row r="304">
@@ -37451,7 +37451,7 @@
         <v>0</v>
       </c>
       <c r="AJ304" t="n">
-        <v>1.127708571159135</v>
+        <v>0.9900456379463807</v>
       </c>
     </row>
     <row r="305">
@@ -37569,7 +37569,7 @@
         <v>0</v>
       </c>
       <c r="AJ305" t="n">
-        <v>0.9428329670994249</v>
+        <v>1.267245514791902</v>
       </c>
     </row>
     <row r="306">
@@ -37687,7 +37687,7 @@
         <v>0</v>
       </c>
       <c r="AJ306" t="n">
-        <v>1.32447086792025</v>
+        <v>1.133708134682106</v>
       </c>
     </row>
     <row r="307">
@@ -37809,7 +37809,7 @@
         <v>0</v>
       </c>
       <c r="AJ307" t="n">
-        <v>1.008591158450882</v>
+        <v>1.273870062770279</v>
       </c>
     </row>
     <row r="308">
@@ -37927,7 +37927,7 @@
         <v>0</v>
       </c>
       <c r="AJ308" t="n">
-        <v>0.9170124839134677</v>
+        <v>0.9221116360795545</v>
       </c>
     </row>
     <row r="309">
@@ -38045,7 +38045,7 @@
         <v>0</v>
       </c>
       <c r="AJ309" t="n">
-        <v>0.9490745788363608</v>
+        <v>1.010062865014543</v>
       </c>
     </row>
     <row r="310">
@@ -38167,7 +38167,7 @@
         <v>0</v>
       </c>
       <c r="AJ310" t="n">
-        <v>0.9449413847288219</v>
+        <v>1.28446062457128</v>
       </c>
     </row>
     <row r="311">
@@ -38285,7 +38285,7 @@
         <v>0</v>
       </c>
       <c r="AJ311" t="n">
-        <v>0.8205475564383908</v>
+        <v>0.9782476394427185</v>
       </c>
     </row>
     <row r="312">
@@ -38403,7 +38403,7 @@
         <v>0</v>
       </c>
       <c r="AJ312" t="n">
-        <v>0.8991810550625478</v>
+        <v>0.9744354714920364</v>
       </c>
     </row>
     <row r="313">
@@ -38521,7 +38521,7 @@
         <v>0</v>
       </c>
       <c r="AJ313" t="n">
-        <v>0.871757027913926</v>
+        <v>0.9575361109612367</v>
       </c>
     </row>
     <row r="314">
@@ -38643,7 +38643,7 @@
         <v>0</v>
       </c>
       <c r="AJ314" t="n">
-        <v>1.137774595380197</v>
+        <v>1.118772056832502</v>
       </c>
     </row>
     <row r="315">
@@ -38761,7 +38761,7 @@
         <v>0</v>
       </c>
       <c r="AJ315" t="n">
-        <v>0.7729946975219504</v>
+        <v>0.6745770689866094</v>
       </c>
     </row>
     <row r="316">
@@ -38883,7 +38883,7 @@
         <v>0</v>
       </c>
       <c r="AJ316" t="n">
-        <v>1.026775150073478</v>
+        <v>1.310316456624326</v>
       </c>
     </row>
     <row r="317">
@@ -39001,7 +39001,7 @@
         <v>0</v>
       </c>
       <c r="AJ317" t="n">
-        <v>0.6379368557120759</v>
+        <v>0.413518142907324</v>
       </c>
     </row>
     <row r="318">
@@ -39123,7 +39123,7 @@
         <v>0</v>
       </c>
       <c r="AJ318" t="n">
-        <v>1.154543975337686</v>
+        <v>1.429105203514217</v>
       </c>
     </row>
     <row r="319">
@@ -39241,7 +39241,7 @@
         <v>0</v>
       </c>
       <c r="AJ319" t="n">
-        <v>1.103417198023252</v>
+        <v>1.401253031360503</v>
       </c>
     </row>
     <row r="320">
@@ -39363,7 +39363,7 @@
         <v>0</v>
       </c>
       <c r="AJ320" t="n">
-        <v>1.230408016124561</v>
+        <v>1.591689837836607</v>
       </c>
     </row>
     <row r="321">
@@ -39481,7 +39481,7 @@
         <v>0</v>
       </c>
       <c r="AJ321" t="n">
-        <v>0.8973524644400391</v>
+        <v>1.151187888149562</v>
       </c>
     </row>
     <row r="322">
@@ -39599,7 +39599,7 @@
         <v>0</v>
       </c>
       <c r="AJ322" t="n">
-        <v>1.032992015777296</v>
+        <v>1.363457827992447</v>
       </c>
     </row>
     <row r="323">
@@ -39721,7 +39721,7 @@
         <v>0</v>
       </c>
       <c r="AJ323" t="n">
-        <v>0.8937173703197223</v>
+        <v>1.077222699601204</v>
       </c>
     </row>
     <row r="324">
@@ -39839,7 +39839,7 @@
         <v>0</v>
       </c>
       <c r="AJ324" t="n">
-        <v>1.142179999213882</v>
+        <v>0.9742993328105041</v>
       </c>
     </row>
     <row r="325">
@@ -39961,7 +39961,7 @@
         <v>0</v>
       </c>
       <c r="AJ325" t="n">
-        <v>0.9511631668430977</v>
+        <v>1.105952557467382</v>
       </c>
     </row>
     <row r="326">
@@ -40079,7 +40079,7 @@
         <v>0</v>
       </c>
       <c r="AJ326" t="n">
-        <v>1.176378407280026</v>
+        <v>1.282468755131865</v>
       </c>
     </row>
     <row r="327">
@@ -40197,7 +40197,7 @@
         <v>0</v>
       </c>
       <c r="AJ327" t="n">
-        <v>0.8199408022148571</v>
+        <v>1.434803328086182</v>
       </c>
     </row>
     <row r="328">
@@ -40319,7 +40319,7 @@
         <v>0</v>
       </c>
       <c r="AJ328" t="n">
-        <v>0.9995772510981604</v>
+        <v>1.409423902881426</v>
       </c>
     </row>
     <row r="329">
@@ -40441,7 +40441,7 @@
         <v>0</v>
       </c>
       <c r="AJ329" t="n">
-        <v>0.897500106027917</v>
+        <v>0.9483123032967564</v>
       </c>
     </row>
     <row r="330">
@@ -40563,7 +40563,7 @@
         <v>0</v>
       </c>
       <c r="AJ330" t="n">
-        <v>1.124043764620542</v>
+        <v>1.313572959454956</v>
       </c>
     </row>
     <row r="331">
@@ -40685,7 +40685,7 @@
         <v>0</v>
       </c>
       <c r="AJ331" t="n">
-        <v>0.8494890585920082</v>
+        <v>0.02427220881691452</v>
       </c>
     </row>
     <row r="332">
@@ -40807,7 +40807,7 @@
         <v>0</v>
       </c>
       <c r="AJ332" t="n">
-        <v>1.463036674509546</v>
+        <v>1.582341434489243</v>
       </c>
     </row>
     <row r="333">
@@ -40925,7 +40925,7 @@
         <v>0</v>
       </c>
       <c r="AJ333" t="n">
-        <v>1.171157574796366</v>
+        <v>1.095377518818988</v>
       </c>
     </row>
     <row r="334">
@@ -41043,7 +41043,7 @@
         <v>0</v>
       </c>
       <c r="AJ334" t="n">
-        <v>1.081986820794462</v>
+        <v>1.223739160525019</v>
       </c>
     </row>
     <row r="335">
@@ -41165,7 +41165,7 @@
         <v>0</v>
       </c>
       <c r="AJ335" t="n">
-        <v>0.703240823557347</v>
+        <v>0.0200951778159242</v>
       </c>
     </row>
     <row r="336">
@@ -41283,7 +41283,7 @@
         <v>0</v>
       </c>
       <c r="AJ336" t="n">
-        <v>0.9237221094625508</v>
+        <v>1.256137369113409</v>
       </c>
     </row>
     <row r="337">
@@ -41405,7 +41405,7 @@
         <v>0</v>
       </c>
       <c r="AJ337" t="n">
-        <v>1.527889104878332</v>
+        <v>1.290033378127408</v>
       </c>
     </row>
     <row r="338">
@@ -41523,7 +41523,7 @@
         <v>0</v>
       </c>
       <c r="AJ338" t="n">
-        <v>1.327158390976689</v>
+        <v>1.132665608277857</v>
       </c>
     </row>
     <row r="339">
@@ -41641,7 +41641,7 @@
         <v>0</v>
       </c>
       <c r="AJ339" t="n">
-        <v>0.8841658429246106</v>
+        <v>1.040192660818712</v>
       </c>
     </row>
     <row r="340">
@@ -41763,7 +41763,7 @@
         <v>0</v>
       </c>
       <c r="AJ340" t="n">
-        <v>1.060906233478993</v>
+        <v>1.045242421977408</v>
       </c>
     </row>
     <row r="341">
@@ -41881,7 +41881,7 @@
         <v>0</v>
       </c>
       <c r="AJ341" t="n">
-        <v>1.34597401850218</v>
+        <v>1.319436408579432</v>
       </c>
     </row>
     <row r="342">
@@ -42003,7 +42003,7 @@
         <v>0</v>
       </c>
       <c r="AJ342" t="n">
-        <v>1.282275062944348</v>
+        <v>1.268484400112522</v>
       </c>
     </row>
     <row r="343">
@@ -42125,7 +42125,7 @@
         <v>0</v>
       </c>
       <c r="AJ343" t="n">
-        <v>1.077135880559634</v>
+        <v>1.128290437895118</v>
       </c>
     </row>
     <row r="344">
@@ -42247,7 +42247,7 @@
         <v>0</v>
       </c>
       <c r="AJ344" t="n">
-        <v>1.398459569953176</v>
+        <v>1.204219517640636</v>
       </c>
     </row>
     <row r="345">
@@ -42365,7 +42365,7 @@
         <v>0</v>
       </c>
       <c r="AJ345" t="n">
-        <v>0.8470456484249165</v>
+        <v>1.216565394838555</v>
       </c>
     </row>
     <row r="346">
@@ -42487,7 +42487,7 @@
         <v>0</v>
       </c>
       <c r="AJ346" t="n">
-        <v>1.052514408312166</v>
+        <v>1.237820737370003</v>
       </c>
     </row>
     <row r="347">
@@ -42609,7 +42609,7 @@
         <v>0</v>
       </c>
       <c r="AJ347" t="n">
-        <v>1.131141622096895</v>
+        <v>1.226092789697735</v>
       </c>
     </row>
     <row r="348">
@@ -42731,7 +42731,7 @@
         <v>0</v>
       </c>
       <c r="AJ348" t="n">
-        <v>1.193444131486028</v>
+        <v>1.190080498790886</v>
       </c>
     </row>
     <row r="349">
@@ -42853,7 +42853,7 @@
         <v>0</v>
       </c>
       <c r="AJ349" t="n">
-        <v>1.299406735033347</v>
+        <v>1.424167694289274</v>
       </c>
     </row>
     <row r="350">
@@ -42971,7 +42971,7 @@
         <v>0</v>
       </c>
       <c r="AJ350" t="n">
-        <v>1.05418819431277</v>
+        <v>1.306203625197601</v>
       </c>
     </row>
     <row r="351">
@@ -43089,7 +43089,7 @@
         <v>0</v>
       </c>
       <c r="AJ351" t="n">
-        <v>0.9045795386334662</v>
+        <v>0.9748868479888309</v>
       </c>
     </row>
     <row r="352">
@@ -43211,7 +43211,7 @@
         <v>0</v>
       </c>
       <c r="AJ352" t="n">
-        <v>1.048940366356069</v>
+        <v>1.2715828239453</v>
       </c>
     </row>
     <row r="353">
@@ -43333,7 +43333,7 @@
         <v>0</v>
       </c>
       <c r="AJ353" t="n">
-        <v>0.6231376102105394</v>
+        <v>0.01780480457744398</v>
       </c>
     </row>
     <row r="354">
@@ -43451,7 +43451,7 @@
         <v>0</v>
       </c>
       <c r="AJ354" t="n">
-        <v>1.075291376355997</v>
+        <v>0.9497187325339085</v>
       </c>
     </row>
     <row r="355">
@@ -43573,7 +43573,7 @@
         <v>0</v>
       </c>
       <c r="AJ355" t="n">
-        <v>0.5561205412664756</v>
+        <v>0.0158894883218993</v>
       </c>
     </row>
     <row r="356">
@@ -43695,7 +43695,7 @@
         <v>0</v>
       </c>
       <c r="AJ356" t="n">
-        <v>1.165488191789052</v>
+        <v>1.155249967122186</v>
       </c>
     </row>
     <row r="357">
@@ -43817,7 +43817,7 @@
         <v>0</v>
       </c>
       <c r="AJ357" t="n">
-        <v>0.8905901205446917</v>
+        <v>0.9618133084797293</v>
       </c>
     </row>
     <row r="358">
@@ -43935,7 +43935,7 @@
         <v>0</v>
       </c>
       <c r="AJ358" t="n">
-        <v>1.379075510428788</v>
+        <v>1.147195439870087</v>
       </c>
     </row>
     <row r="359">
@@ -44057,7 +44057,7 @@
         <v>0</v>
       </c>
       <c r="AJ359" t="n">
-        <v>0.9215947321849139</v>
+        <v>0.978304222930951</v>
       </c>
     </row>
     <row r="360">
@@ -44179,7 +44179,7 @@
         <v>0</v>
       </c>
       <c r="AJ360" t="n">
-        <v>1.969545964764595</v>
+        <v>1.452364691648306</v>
       </c>
     </row>
     <row r="361">
@@ -44301,7 +44301,7 @@
         <v>0</v>
       </c>
       <c r="AJ361" t="n">
-        <v>1.597551554389408</v>
+        <v>1.181301414604549</v>
       </c>
     </row>
     <row r="362">
@@ -44419,7 +44419,7 @@
         <v>0</v>
       </c>
       <c r="AJ362" t="n">
-        <v>0.9232748998256796</v>
+        <v>1.119312244843634</v>
       </c>
     </row>
     <row r="363">
@@ -44541,7 +44541,7 @@
         <v>0</v>
       </c>
       <c r="AJ363" t="n">
-        <v>1.012432006260436</v>
+        <v>1.241206030877317</v>
       </c>
     </row>
     <row r="364">
@@ -44663,7 +44663,7 @@
         <v>0</v>
       </c>
       <c r="AJ364" t="n">
-        <v>1.164768709137029</v>
+        <v>1.596629881899644</v>
       </c>
     </row>
     <row r="365">
@@ -44785,7 +44785,7 @@
         <v>0</v>
       </c>
       <c r="AJ365" t="n">
-        <v>1.030015139472722</v>
+        <v>1.10814143447182</v>
       </c>
     </row>
     <row r="366">
@@ -44907,7 +44907,7 @@
         <v>0</v>
       </c>
       <c r="AJ366" t="n">
-        <v>0.8617900020651388</v>
+        <v>1.018858819896442</v>
       </c>
     </row>
     <row r="367">
@@ -45025,7 +45025,7 @@
         <v>0</v>
       </c>
       <c r="AJ367" t="n">
-        <v>0.8700725000497508</v>
+        <v>0.9630209690648511</v>
       </c>
     </row>
     <row r="368">
@@ -45143,7 +45143,7 @@
         <v>0</v>
       </c>
       <c r="AJ368" t="n">
-        <v>1.045742553809369</v>
+        <v>0.9781916970497975</v>
       </c>
     </row>
     <row r="369">
@@ -45261,7 +45261,7 @@
         <v>0</v>
       </c>
       <c r="AJ369" t="n">
-        <v>1.118791091281928</v>
+        <v>0.4337267146760114</v>
       </c>
     </row>
     <row r="370">
@@ -45383,7 +45383,7 @@
         <v>0</v>
       </c>
       <c r="AJ370" t="n">
-        <v>0.5971296682419419</v>
+        <v>0.01706348052119834</v>
       </c>
     </row>
     <row r="371">
@@ -45505,7 +45505,7 @@
         <v>0</v>
       </c>
       <c r="AJ371" t="n">
-        <v>0.9787998080303336</v>
+        <v>1.161680123149465</v>
       </c>
     </row>
     <row r="372">
@@ -45627,7 +45627,7 @@
         <v>0</v>
       </c>
       <c r="AJ372" t="n">
-        <v>0.9372363418753887</v>
+        <v>1.166993487390219</v>
       </c>
     </row>
     <row r="373">
@@ -45745,7 +45745,7 @@
         <v>0</v>
       </c>
       <c r="AJ373" t="n">
-        <v>1.1268634064606</v>
+        <v>1.767129014303091</v>
       </c>
     </row>
     <row r="374">
@@ -45867,7 +45867,7 @@
         <v>0</v>
       </c>
       <c r="AJ374" t="n">
-        <v>0.4934557400469028</v>
+        <v>0.01409944114419722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>